<commit_message>
Use euclidean distance for registration scoring, disable progress bar
</commit_message>
<xml_diff>
--- a/Database/CoastSnapPyDB.xlsx
+++ b/Database/CoastSnapPyDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\CoastSnap\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0858465-45C7-4108-AF12-4723710FF265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F4C1CF7-834E-4E6B-808E-C952F27D4D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1396" uniqueCount="375">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1480" uniqueCount="389">
   <si>
     <t>Site</t>
   </si>
@@ -1164,6 +1164,48 @@
   </si>
   <si>
     <t>detection_model-ex-009--loss-0012.315.h5</t>
+  </si>
+  <si>
+    <t>target20.jpg</t>
+  </si>
+  <si>
+    <t>target18.jpg</t>
+  </si>
+  <si>
+    <t>target26.jpg</t>
+  </si>
+  <si>
+    <t>target23.jpg</t>
+  </si>
+  <si>
+    <t>target19.jpg</t>
+  </si>
+  <si>
+    <t>target24.jpg</t>
+  </si>
+  <si>
+    <t>target21.jpg</t>
+  </si>
+  <si>
+    <t>target32.jpg</t>
+  </si>
+  <si>
+    <t>target30.jpg</t>
+  </si>
+  <si>
+    <t>target27.jpg</t>
+  </si>
+  <si>
+    <t>target33.jpg</t>
+  </si>
+  <si>
+    <t>target25.jpg</t>
+  </si>
+  <si>
+    <t>target28.jpg</t>
+  </si>
+  <si>
+    <t>target22.jpg</t>
   </si>
 </sst>
 </file>
@@ -1597,11 +1639,41 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="15" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1614,36 +1686,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -20609,8 +20651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82C2A5-FA5F-4BBC-B066-D9DA22911E90}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="M66" sqref="M66"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="B130" sqref="B130:D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -20629,18 +20671,18 @@
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="41"/>
-      <c r="D1" s="126"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="128"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="93"/>
+      <c r="F1" s="93"/>
+      <c r="G1" s="93"/>
+      <c r="H1" s="93"/>
+      <c r="I1" s="93"/>
+      <c r="J1" s="93"/>
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="94"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
@@ -20661,20 +20703,20 @@
       <c r="C2" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="D2" s="129" t="s">
+      <c r="D2" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="130"/>
-      <c r="L2" s="130"/>
-      <c r="M2" s="130"/>
-      <c r="N2" s="130"/>
-      <c r="O2" s="131"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="96"/>
+      <c r="I2" s="96"/>
+      <c r="J2" s="96"/>
+      <c r="K2" s="96"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="97"/>
       <c r="P2" s="3"/>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
@@ -20695,20 +20737,20 @@
       <c r="C3" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="129" t="s">
+      <c r="D3" s="95" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="130"/>
-      <c r="F3" s="130"/>
-      <c r="G3" s="130"/>
-      <c r="H3" s="130"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
-      <c r="N3" s="130"/>
-      <c r="O3" s="131"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
+      <c r="H3" s="96"/>
+      <c r="I3" s="96"/>
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
@@ -20729,20 +20771,20 @@
       <c r="C4" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="D4" s="129" t="s">
+      <c r="D4" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="E4" s="130"/>
-      <c r="F4" s="130"/>
-      <c r="G4" s="130"/>
-      <c r="H4" s="130"/>
-      <c r="I4" s="130"/>
-      <c r="J4" s="130"/>
-      <c r="K4" s="130"/>
-      <c r="L4" s="130"/>
-      <c r="M4" s="130"/>
-      <c r="N4" s="130"/>
-      <c r="O4" s="131"/>
+      <c r="E4" s="96"/>
+      <c r="F4" s="96"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="96"/>
+      <c r="I4" s="96"/>
+      <c r="J4" s="96"/>
+      <c r="K4" s="96"/>
+      <c r="L4" s="96"/>
+      <c r="M4" s="96"/>
+      <c r="N4" s="96"/>
+      <c r="O4" s="97"/>
       <c r="P4" s="3"/>
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
@@ -20761,20 +20803,20 @@
         <v>125</v>
       </c>
       <c r="C5" s="43"/>
-      <c r="D5" s="129" t="s">
+      <c r="D5" s="95" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="130"/>
-      <c r="F5" s="130"/>
-      <c r="G5" s="130"/>
-      <c r="H5" s="130"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="130"/>
-      <c r="K5" s="130"/>
-      <c r="L5" s="130"/>
-      <c r="M5" s="130"/>
-      <c r="N5" s="130"/>
-      <c r="O5" s="131"/>
+      <c r="E5" s="96"/>
+      <c r="F5" s="96"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="96"/>
+      <c r="K5" s="96"/>
+      <c r="L5" s="96"/>
+      <c r="M5" s="96"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="97"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3"/>
       <c r="R5" s="3"/>
@@ -20795,20 +20837,20 @@
       <c r="C6" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="129" t="s">
+      <c r="D6" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="130"/>
-      <c r="F6" s="130"/>
-      <c r="G6" s="130"/>
-      <c r="H6" s="130"/>
-      <c r="I6" s="130"/>
-      <c r="J6" s="130"/>
-      <c r="K6" s="130"/>
-      <c r="L6" s="130"/>
-      <c r="M6" s="130"/>
-      <c r="N6" s="130"/>
-      <c r="O6" s="131"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
+      <c r="J6" s="96"/>
+      <c r="K6" s="96"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="96"/>
+      <c r="N6" s="96"/>
+      <c r="O6" s="97"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3"/>
       <c r="R6" s="3"/>
@@ -20829,20 +20871,20 @@
       <c r="C7" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="129" t="s">
+      <c r="D7" s="95" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="130"/>
-      <c r="F7" s="130"/>
-      <c r="G7" s="130"/>
-      <c r="H7" s="130"/>
-      <c r="I7" s="130"/>
-      <c r="J7" s="130"/>
-      <c r="K7" s="130"/>
-      <c r="L7" s="130"/>
-      <c r="M7" s="130"/>
-      <c r="N7" s="130"/>
-      <c r="O7" s="131"/>
+      <c r="E7" s="96"/>
+      <c r="F7" s="96"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="96"/>
+      <c r="J7" s="96"/>
+      <c r="K7" s="96"/>
+      <c r="L7" s="96"/>
+      <c r="M7" s="96"/>
+      <c r="N7" s="96"/>
+      <c r="O7" s="97"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
@@ -20863,20 +20905,20 @@
       <c r="C8" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="129" t="s">
+      <c r="D8" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="130"/>
-      <c r="F8" s="130"/>
-      <c r="G8" s="130"/>
-      <c r="H8" s="130"/>
-      <c r="I8" s="130"/>
-      <c r="J8" s="130"/>
-      <c r="K8" s="130"/>
-      <c r="L8" s="130"/>
-      <c r="M8" s="130"/>
-      <c r="N8" s="130"/>
-      <c r="O8" s="131"/>
+      <c r="E8" s="96"/>
+      <c r="F8" s="96"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+      <c r="I8" s="96"/>
+      <c r="J8" s="96"/>
+      <c r="K8" s="96"/>
+      <c r="L8" s="96"/>
+      <c r="M8" s="96"/>
+      <c r="N8" s="96"/>
+      <c r="O8" s="97"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="3"/>
@@ -20897,20 +20939,20 @@
       <c r="C9" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="129" t="s">
+      <c r="D9" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="E9" s="130"/>
-      <c r="F9" s="130"/>
-      <c r="G9" s="130"/>
-      <c r="H9" s="130"/>
-      <c r="I9" s="130"/>
-      <c r="J9" s="130"/>
-      <c r="K9" s="130"/>
-      <c r="L9" s="130"/>
-      <c r="M9" s="130"/>
-      <c r="N9" s="130"/>
-      <c r="O9" s="131"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="97"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
@@ -20927,18 +20969,18 @@
       </c>
       <c r="B10" s="46"/>
       <c r="C10" s="47"/>
-      <c r="D10" s="120"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="121"/>
-      <c r="I10" s="121"/>
-      <c r="J10" s="121"/>
-      <c r="K10" s="121"/>
-      <c r="L10" s="121"/>
-      <c r="M10" s="121"/>
-      <c r="N10" s="121"/>
-      <c r="O10" s="122"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="99"/>
+      <c r="N10" s="99"/>
+      <c r="O10" s="100"/>
       <c r="P10" s="48"/>
       <c r="Q10" s="48"/>
       <c r="R10" s="48"/>
@@ -20959,20 +21001,20 @@
       <c r="C11" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="117" t="s">
+      <c r="D11" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="118"/>
-      <c r="F11" s="118"/>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="118"/>
-      <c r="O11" s="119"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="90"/>
+      <c r="G11" s="90"/>
+      <c r="H11" s="90"/>
+      <c r="I11" s="90"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="90"/>
+      <c r="L11" s="90"/>
+      <c r="M11" s="90"/>
+      <c r="N11" s="90"/>
+      <c r="O11" s="91"/>
       <c r="P11" s="48"/>
       <c r="Q11" s="48"/>
       <c r="R11" s="48"/>
@@ -20993,20 +21035,20 @@
       <c r="C12" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="117" t="s">
+      <c r="D12" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
-      <c r="I12" s="118"/>
-      <c r="J12" s="118"/>
-      <c r="K12" s="118"/>
-      <c r="L12" s="118"/>
-      <c r="M12" s="118"/>
-      <c r="N12" s="118"/>
-      <c r="O12" s="119"/>
+      <c r="E12" s="90"/>
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="90"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
+      <c r="N12" s="90"/>
+      <c r="O12" s="91"/>
       <c r="P12" s="48"/>
       <c r="Q12" s="48"/>
       <c r="R12" s="48"/>
@@ -21027,20 +21069,20 @@
       <c r="C13" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="117" t="s">
+      <c r="D13" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
-      <c r="I13" s="118"/>
-      <c r="J13" s="118"/>
-      <c r="K13" s="118"/>
-      <c r="L13" s="118"/>
-      <c r="M13" s="118"/>
-      <c r="N13" s="118"/>
-      <c r="O13" s="119"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="90"/>
+      <c r="H13" s="90"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
+      <c r="M13" s="90"/>
+      <c r="N13" s="90"/>
+      <c r="O13" s="91"/>
       <c r="P13" s="48"/>
       <c r="Q13" s="48"/>
       <c r="R13" s="48"/>
@@ -21061,20 +21103,20 @@
       <c r="C14" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="117" t="s">
+      <c r="D14" s="89" t="s">
         <v>82</v>
       </c>
-      <c r="E14" s="118"/>
-      <c r="F14" s="118"/>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
-      <c r="I14" s="118"/>
-      <c r="J14" s="118"/>
-      <c r="K14" s="118"/>
-      <c r="L14" s="118"/>
-      <c r="M14" s="118"/>
-      <c r="N14" s="118"/>
-      <c r="O14" s="119"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
+      <c r="H14" s="90"/>
+      <c r="I14" s="90"/>
+      <c r="J14" s="90"/>
+      <c r="K14" s="90"/>
+      <c r="L14" s="90"/>
+      <c r="M14" s="90"/>
+      <c r="N14" s="90"/>
+      <c r="O14" s="91"/>
       <c r="P14" s="48"/>
       <c r="Q14" s="48"/>
       <c r="R14" s="48"/>
@@ -21095,20 +21137,20 @@
       <c r="C15" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="117" t="s">
+      <c r="D15" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="E15" s="118"/>
-      <c r="F15" s="118"/>
-      <c r="G15" s="118"/>
-      <c r="H15" s="118"/>
-      <c r="I15" s="118"/>
-      <c r="J15" s="118"/>
-      <c r="K15" s="118"/>
-      <c r="L15" s="118"/>
-      <c r="M15" s="118"/>
-      <c r="N15" s="118"/>
-      <c r="O15" s="119"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90"/>
+      <c r="I15" s="90"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="90"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="90"/>
+      <c r="N15" s="90"/>
+      <c r="O15" s="91"/>
       <c r="P15" s="48"/>
       <c r="Q15" s="48"/>
       <c r="R15" s="48"/>
@@ -21129,20 +21171,20 @@
       <c r="C16" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="117" t="s">
+      <c r="D16" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
-      <c r="G16" s="118"/>
-      <c r="H16" s="118"/>
-      <c r="I16" s="118"/>
-      <c r="J16" s="118"/>
-      <c r="K16" s="118"/>
-      <c r="L16" s="118"/>
-      <c r="M16" s="118"/>
-      <c r="N16" s="118"/>
-      <c r="O16" s="119"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="90"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="90"/>
+      <c r="L16" s="90"/>
+      <c r="M16" s="90"/>
+      <c r="N16" s="90"/>
+      <c r="O16" s="91"/>
       <c r="P16" s="48"/>
       <c r="Q16" s="48"/>
       <c r="R16" s="48"/>
@@ -21163,20 +21205,20 @@
       <c r="C17" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="117" t="s">
+      <c r="D17" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="E17" s="118"/>
-      <c r="F17" s="118"/>
-      <c r="G17" s="118"/>
-      <c r="H17" s="118"/>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
-      <c r="N17" s="118"/>
-      <c r="O17" s="119"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+      <c r="G17" s="90"/>
+      <c r="H17" s="90"/>
+      <c r="I17" s="90"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="90"/>
+      <c r="L17" s="90"/>
+      <c r="M17" s="90"/>
+      <c r="N17" s="90"/>
+      <c r="O17" s="91"/>
       <c r="P17" s="48"/>
       <c r="Q17" s="48"/>
       <c r="R17" s="48"/>
@@ -21197,20 +21239,20 @@
       <c r="C18" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="117" t="s">
+      <c r="D18" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="E18" s="118"/>
-      <c r="F18" s="118"/>
-      <c r="G18" s="118"/>
-      <c r="H18" s="118"/>
-      <c r="I18" s="118"/>
-      <c r="J18" s="118"/>
-      <c r="K18" s="118"/>
-      <c r="L18" s="118"/>
-      <c r="M18" s="118"/>
-      <c r="N18" s="118"/>
-      <c r="O18" s="119"/>
+      <c r="E18" s="90"/>
+      <c r="F18" s="90"/>
+      <c r="G18" s="90"/>
+      <c r="H18" s="90"/>
+      <c r="I18" s="90"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="91"/>
       <c r="P18" s="82"/>
       <c r="Q18" s="82"/>
       <c r="R18" s="82"/>
@@ -21233,20 +21275,20 @@
       <c r="C19" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="120" t="s">
+      <c r="D19" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="121"/>
-      <c r="F19" s="121"/>
-      <c r="G19" s="121"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="121"/>
-      <c r="J19" s="121"/>
-      <c r="K19" s="121"/>
-      <c r="L19" s="121"/>
-      <c r="M19" s="121"/>
-      <c r="N19" s="121"/>
-      <c r="O19" s="122"/>
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="99"/>
+      <c r="N19" s="99"/>
+      <c r="O19" s="100"/>
       <c r="P19" s="82"/>
       <c r="Q19" s="82"/>
       <c r="R19" s="82"/>
@@ -21269,20 +21311,20 @@
       <c r="C20" s="47" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="120" t="s">
+      <c r="D20" s="98" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="121"/>
-      <c r="F20" s="121"/>
-      <c r="G20" s="121"/>
-      <c r="H20" s="121"/>
-      <c r="I20" s="121"/>
-      <c r="J20" s="121"/>
-      <c r="K20" s="121"/>
-      <c r="L20" s="121"/>
-      <c r="M20" s="121"/>
-      <c r="N20" s="121"/>
-      <c r="O20" s="122"/>
+      <c r="E20" s="99"/>
+      <c r="F20" s="99"/>
+      <c r="G20" s="99"/>
+      <c r="H20" s="99"/>
+      <c r="I20" s="99"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="99"/>
+      <c r="M20" s="99"/>
+      <c r="N20" s="99"/>
+      <c r="O20" s="100"/>
       <c r="P20" s="82"/>
       <c r="Q20" s="82"/>
       <c r="R20" s="82"/>
@@ -21305,20 +21347,20 @@
       <c r="C21" s="47" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="120" t="s">
+      <c r="D21" s="98" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="121"/>
-      <c r="F21" s="121"/>
-      <c r="G21" s="121"/>
-      <c r="H21" s="121"/>
-      <c r="I21" s="121"/>
-      <c r="J21" s="121"/>
-      <c r="K21" s="121"/>
-      <c r="L21" s="121"/>
-      <c r="M21" s="121"/>
-      <c r="N21" s="121"/>
-      <c r="O21" s="122"/>
+      <c r="E21" s="99"/>
+      <c r="F21" s="99"/>
+      <c r="G21" s="99"/>
+      <c r="H21" s="99"/>
+      <c r="I21" s="99"/>
+      <c r="J21" s="99"/>
+      <c r="K21" s="99"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="99"/>
+      <c r="N21" s="99"/>
+      <c r="O21" s="100"/>
       <c r="P21" s="82"/>
       <c r="Q21" s="82"/>
       <c r="R21" s="82"/>
@@ -21341,20 +21383,20 @@
       <c r="C22" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="117" t="s">
+      <c r="D22" s="89" t="s">
         <v>118</v>
       </c>
-      <c r="E22" s="118"/>
-      <c r="F22" s="118"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="118"/>
-      <c r="I22" s="118"/>
-      <c r="J22" s="118"/>
-      <c r="K22" s="118"/>
-      <c r="L22" s="118"/>
-      <c r="M22" s="118"/>
-      <c r="N22" s="118"/>
-      <c r="O22" s="119"/>
+      <c r="E22" s="90"/>
+      <c r="F22" s="90"/>
+      <c r="G22" s="90"/>
+      <c r="H22" s="90"/>
+      <c r="I22" s="90"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="90"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="91"/>
       <c r="P22" s="82"/>
       <c r="Q22" s="82"/>
       <c r="R22" s="82"/>
@@ -21373,18 +21415,18 @@
       </c>
       <c r="B23" s="11"/>
       <c r="C23" s="11"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="124"/>
-      <c r="F23" s="124"/>
-      <c r="G23" s="124"/>
-      <c r="H23" s="124"/>
-      <c r="I23" s="124"/>
-      <c r="J23" s="124"/>
-      <c r="K23" s="124"/>
-      <c r="L23" s="124"/>
-      <c r="M23" s="124"/>
-      <c r="N23" s="124"/>
-      <c r="O23" s="125"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105"/>
+      <c r="H23" s="105"/>
+      <c r="I23" s="105"/>
+      <c r="J23" s="105"/>
+      <c r="K23" s="105"/>
+      <c r="L23" s="105"/>
+      <c r="M23" s="105"/>
+      <c r="N23" s="105"/>
+      <c r="O23" s="106"/>
       <c r="P23" s="84"/>
       <c r="Q23" s="84"/>
       <c r="R23" s="84"/>
@@ -21405,20 +21447,20 @@
         <v>323</v>
       </c>
       <c r="C24" s="50"/>
-      <c r="D24" s="102" t="s">
+      <c r="D24" s="101" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103"/>
-      <c r="G24" s="103"/>
-      <c r="H24" s="103"/>
-      <c r="I24" s="103"/>
-      <c r="J24" s="103"/>
-      <c r="K24" s="103"/>
-      <c r="L24" s="103"/>
-      <c r="M24" s="103"/>
-      <c r="N24" s="103"/>
-      <c r="O24" s="104"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="103"/>
       <c r="P24" s="84"/>
       <c r="Q24" s="84"/>
       <c r="R24" s="84"/>
@@ -21441,20 +21483,20 @@
       <c r="C25" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="102" t="s">
+      <c r="D25" s="101" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="103"/>
-      <c r="F25" s="103"/>
-      <c r="G25" s="103"/>
-      <c r="H25" s="103"/>
-      <c r="I25" s="103"/>
-      <c r="J25" s="103"/>
-      <c r="K25" s="103"/>
-      <c r="L25" s="103"/>
-      <c r="M25" s="103"/>
-      <c r="N25" s="103"/>
-      <c r="O25" s="104"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="103"/>
       <c r="P25" s="84"/>
       <c r="Q25" s="84"/>
       <c r="R25" s="84"/>
@@ -21473,18 +21515,18 @@
       </c>
       <c r="B26" s="18"/>
       <c r="C26" s="18"/>
-      <c r="D26" s="105"/>
-      <c r="E26" s="106"/>
-      <c r="F26" s="106"/>
-      <c r="G26" s="106"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="106"/>
-      <c r="J26" s="106"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="106"/>
-      <c r="N26" s="106"/>
-      <c r="O26" s="107"/>
+      <c r="D26" s="110"/>
+      <c r="E26" s="111"/>
+      <c r="F26" s="111"/>
+      <c r="G26" s="111"/>
+      <c r="H26" s="111"/>
+      <c r="I26" s="111"/>
+      <c r="J26" s="111"/>
+      <c r="K26" s="111"/>
+      <c r="L26" s="111"/>
+      <c r="M26" s="111"/>
+      <c r="N26" s="111"/>
+      <c r="O26" s="112"/>
       <c r="P26" s="85"/>
       <c r="Q26" s="85"/>
       <c r="R26" s="85"/>
@@ -21505,20 +21547,20 @@
         <v>325</v>
       </c>
       <c r="C27" s="53"/>
-      <c r="D27" s="108" t="s">
+      <c r="D27" s="113" t="s">
         <v>98</v>
       </c>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="109"/>
-      <c r="O27" s="110"/>
+      <c r="E27" s="114"/>
+      <c r="F27" s="114"/>
+      <c r="G27" s="114"/>
+      <c r="H27" s="114"/>
+      <c r="I27" s="114"/>
+      <c r="J27" s="114"/>
+      <c r="K27" s="114"/>
+      <c r="L27" s="114"/>
+      <c r="M27" s="114"/>
+      <c r="N27" s="114"/>
+      <c r="O27" s="115"/>
       <c r="P27" s="85"/>
       <c r="Q27" s="85"/>
       <c r="R27" s="85"/>
@@ -21539,20 +21581,20 @@
         <v>72</v>
       </c>
       <c r="C28" s="53"/>
-      <c r="D28" s="111" t="s">
+      <c r="D28" s="116" t="s">
         <v>96</v>
       </c>
-      <c r="E28" s="112"/>
-      <c r="F28" s="112"/>
-      <c r="G28" s="112"/>
-      <c r="H28" s="112"/>
-      <c r="I28" s="112"/>
-      <c r="J28" s="112"/>
-      <c r="K28" s="112"/>
-      <c r="L28" s="112"/>
-      <c r="M28" s="112"/>
-      <c r="N28" s="112"/>
-      <c r="O28" s="113"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="117"/>
+      <c r="M28" s="117"/>
+      <c r="N28" s="117"/>
+      <c r="O28" s="118"/>
       <c r="P28" s="85"/>
       <c r="Q28" s="85"/>
       <c r="R28" s="85"/>
@@ -21573,20 +21615,20 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C29" s="53"/>
-      <c r="D29" s="111" t="s">
+      <c r="D29" s="116" t="s">
         <v>97</v>
       </c>
-      <c r="E29" s="112"/>
-      <c r="F29" s="112"/>
-      <c r="G29" s="112"/>
-      <c r="H29" s="112"/>
-      <c r="I29" s="112"/>
-      <c r="J29" s="112"/>
-      <c r="K29" s="112"/>
-      <c r="L29" s="112"/>
-      <c r="M29" s="112"/>
-      <c r="N29" s="112"/>
-      <c r="O29" s="113"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="117"/>
+      <c r="I29" s="117"/>
+      <c r="J29" s="117"/>
+      <c r="K29" s="117"/>
+      <c r="L29" s="117"/>
+      <c r="M29" s="117"/>
+      <c r="N29" s="117"/>
+      <c r="O29" s="118"/>
       <c r="P29" s="85"/>
       <c r="Q29" s="85"/>
       <c r="R29" s="85"/>
@@ -21605,20 +21647,20 @@
       </c>
       <c r="B30" s="56"/>
       <c r="C30" s="57"/>
-      <c r="D30" s="114" t="s">
+      <c r="D30" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="E30" s="115"/>
-      <c r="F30" s="115"/>
-      <c r="G30" s="115"/>
-      <c r="H30" s="115"/>
-      <c r="I30" s="115"/>
-      <c r="J30" s="115"/>
-      <c r="K30" s="115"/>
-      <c r="L30" s="115"/>
-      <c r="M30" s="115"/>
-      <c r="N30" s="115"/>
-      <c r="O30" s="116"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="120"/>
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="120"/>
+      <c r="N30" s="120"/>
+      <c r="O30" s="121"/>
       <c r="P30" s="86"/>
       <c r="Q30" s="86"/>
       <c r="R30" s="86"/>
@@ -21639,20 +21681,20 @@
         <v>219</v>
       </c>
       <c r="C31" s="57"/>
-      <c r="D31" s="91" t="s">
+      <c r="D31" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="92"/>
-      <c r="F31" s="92"/>
-      <c r="G31" s="92"/>
-      <c r="H31" s="92"/>
-      <c r="I31" s="92"/>
-      <c r="J31" s="92"/>
-      <c r="K31" s="92"/>
-      <c r="L31" s="92"/>
-      <c r="M31" s="92"/>
-      <c r="N31" s="92"/>
-      <c r="O31" s="93"/>
+      <c r="E31" s="108"/>
+      <c r="F31" s="108"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="108"/>
+      <c r="I31" s="108"/>
+      <c r="J31" s="108"/>
+      <c r="K31" s="108"/>
+      <c r="L31" s="108"/>
+      <c r="M31" s="108"/>
+      <c r="N31" s="108"/>
+      <c r="O31" s="109"/>
       <c r="P31" s="86"/>
       <c r="Q31" s="86"/>
       <c r="R31" s="86"/>
@@ -21675,20 +21717,20 @@
       <c r="C32" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D32" s="91" t="s">
+      <c r="D32" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="92"/>
-      <c r="F32" s="92"/>
-      <c r="G32" s="92"/>
-      <c r="H32" s="92"/>
-      <c r="I32" s="92"/>
-      <c r="J32" s="92"/>
-      <c r="K32" s="92"/>
-      <c r="L32" s="92"/>
-      <c r="M32" s="92"/>
-      <c r="N32" s="92"/>
-      <c r="O32" s="93"/>
+      <c r="E32" s="108"/>
+      <c r="F32" s="108"/>
+      <c r="G32" s="108"/>
+      <c r="H32" s="108"/>
+      <c r="I32" s="108"/>
+      <c r="J32" s="108"/>
+      <c r="K32" s="108"/>
+      <c r="L32" s="108"/>
+      <c r="M32" s="108"/>
+      <c r="N32" s="108"/>
+      <c r="O32" s="109"/>
       <c r="P32" s="86"/>
       <c r="Q32" s="86"/>
       <c r="R32" s="86"/>
@@ -21711,20 +21753,20 @@
       <c r="C33" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="91" t="s">
+      <c r="D33" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E33" s="92"/>
-      <c r="F33" s="92"/>
-      <c r="G33" s="92"/>
-      <c r="H33" s="92"/>
-      <c r="I33" s="92"/>
-      <c r="J33" s="92"/>
-      <c r="K33" s="92"/>
-      <c r="L33" s="92"/>
-      <c r="M33" s="92"/>
-      <c r="N33" s="92"/>
-      <c r="O33" s="93"/>
+      <c r="E33" s="108"/>
+      <c r="F33" s="108"/>
+      <c r="G33" s="108"/>
+      <c r="H33" s="108"/>
+      <c r="I33" s="108"/>
+      <c r="J33" s="108"/>
+      <c r="K33" s="108"/>
+      <c r="L33" s="108"/>
+      <c r="M33" s="108"/>
+      <c r="N33" s="108"/>
+      <c r="O33" s="109"/>
       <c r="P33" s="86"/>
       <c r="Q33" s="86"/>
       <c r="R33" s="86"/>
@@ -21747,20 +21789,20 @@
       <c r="C34" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="91" t="s">
+      <c r="D34" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="92"/>
-      <c r="F34" s="92"/>
-      <c r="G34" s="92"/>
-      <c r="H34" s="92"/>
-      <c r="I34" s="92"/>
-      <c r="J34" s="92"/>
-      <c r="K34" s="92"/>
-      <c r="L34" s="92"/>
-      <c r="M34" s="92"/>
-      <c r="N34" s="92"/>
-      <c r="O34" s="93"/>
+      <c r="E34" s="108"/>
+      <c r="F34" s="108"/>
+      <c r="G34" s="108"/>
+      <c r="H34" s="108"/>
+      <c r="I34" s="108"/>
+      <c r="J34" s="108"/>
+      <c r="K34" s="108"/>
+      <c r="L34" s="108"/>
+      <c r="M34" s="108"/>
+      <c r="N34" s="108"/>
+      <c r="O34" s="109"/>
       <c r="P34" s="86"/>
       <c r="Q34" s="86"/>
       <c r="R34" s="86"/>
@@ -21781,20 +21823,20 @@
         <v>220</v>
       </c>
       <c r="C35" s="57"/>
-      <c r="D35" s="91" t="s">
+      <c r="D35" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="E35" s="92"/>
-      <c r="F35" s="92"/>
-      <c r="G35" s="92"/>
-      <c r="H35" s="92"/>
-      <c r="I35" s="92"/>
-      <c r="J35" s="92"/>
-      <c r="K35" s="92"/>
-      <c r="L35" s="92"/>
-      <c r="M35" s="92"/>
-      <c r="N35" s="92"/>
-      <c r="O35" s="93"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="108"/>
+      <c r="I35" s="108"/>
+      <c r="J35" s="108"/>
+      <c r="K35" s="108"/>
+      <c r="L35" s="108"/>
+      <c r="M35" s="108"/>
+      <c r="N35" s="108"/>
+      <c r="O35" s="109"/>
       <c r="P35" s="86"/>
       <c r="Q35" s="86"/>
       <c r="R35" s="86"/>
@@ -21817,20 +21859,20 @@
       <c r="C36" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D36" s="91" t="s">
+      <c r="D36" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E36" s="92"/>
-      <c r="F36" s="92"/>
-      <c r="G36" s="92"/>
-      <c r="H36" s="92"/>
-      <c r="I36" s="92"/>
-      <c r="J36" s="92"/>
-      <c r="K36" s="92"/>
-      <c r="L36" s="92"/>
-      <c r="M36" s="92"/>
-      <c r="N36" s="92"/>
-      <c r="O36" s="93"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="108"/>
+      <c r="I36" s="108"/>
+      <c r="J36" s="108"/>
+      <c r="K36" s="108"/>
+      <c r="L36" s="108"/>
+      <c r="M36" s="108"/>
+      <c r="N36" s="108"/>
+      <c r="O36" s="109"/>
       <c r="P36" s="86"/>
       <c r="Q36" s="86"/>
       <c r="R36" s="86"/>
@@ -21853,20 +21895,20 @@
       <c r="C37" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D37" s="91" t="s">
+      <c r="D37" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E37" s="92"/>
-      <c r="F37" s="92"/>
-      <c r="G37" s="92"/>
-      <c r="H37" s="92"/>
-      <c r="I37" s="92"/>
-      <c r="J37" s="92"/>
-      <c r="K37" s="92"/>
-      <c r="L37" s="92"/>
-      <c r="M37" s="92"/>
-      <c r="N37" s="92"/>
-      <c r="O37" s="93"/>
+      <c r="E37" s="108"/>
+      <c r="F37" s="108"/>
+      <c r="G37" s="108"/>
+      <c r="H37" s="108"/>
+      <c r="I37" s="108"/>
+      <c r="J37" s="108"/>
+      <c r="K37" s="108"/>
+      <c r="L37" s="108"/>
+      <c r="M37" s="108"/>
+      <c r="N37" s="108"/>
+      <c r="O37" s="109"/>
       <c r="P37" s="86"/>
       <c r="Q37" s="86"/>
       <c r="R37" s="86"/>
@@ -21889,20 +21931,20 @@
       <c r="C38" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="D38" s="91" t="s">
+      <c r="D38" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="92"/>
-      <c r="F38" s="92"/>
-      <c r="G38" s="92"/>
-      <c r="H38" s="92"/>
-      <c r="I38" s="92"/>
-      <c r="J38" s="92"/>
-      <c r="K38" s="92"/>
-      <c r="L38" s="92"/>
-      <c r="M38" s="92"/>
-      <c r="N38" s="92"/>
-      <c r="O38" s="93"/>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
+      <c r="H38" s="108"/>
+      <c r="I38" s="108"/>
+      <c r="J38" s="108"/>
+      <c r="K38" s="108"/>
+      <c r="L38" s="108"/>
+      <c r="M38" s="108"/>
+      <c r="N38" s="108"/>
+      <c r="O38" s="109"/>
       <c r="P38" s="86"/>
       <c r="Q38" s="86"/>
       <c r="R38" s="86"/>
@@ -21923,20 +21965,20 @@
         <v>221</v>
       </c>
       <c r="C39" s="56"/>
-      <c r="D39" s="91" t="s">
+      <c r="D39" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="E39" s="92"/>
-      <c r="F39" s="92"/>
-      <c r="G39" s="92"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92"/>
-      <c r="K39" s="92"/>
-      <c r="L39" s="92"/>
-      <c r="M39" s="92"/>
-      <c r="N39" s="92"/>
-      <c r="O39" s="93"/>
+      <c r="E39" s="108"/>
+      <c r="F39" s="108"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="108"/>
+      <c r="I39" s="108"/>
+      <c r="J39" s="108"/>
+      <c r="K39" s="108"/>
+      <c r="L39" s="108"/>
+      <c r="M39" s="108"/>
+      <c r="N39" s="108"/>
+      <c r="O39" s="109"/>
       <c r="P39" s="86"/>
       <c r="Q39" s="86"/>
       <c r="R39" s="86"/>
@@ -21959,20 +22001,20 @@
       <c r="C40" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="91" t="s">
+      <c r="D40" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E40" s="92"/>
-      <c r="F40" s="92"/>
-      <c r="G40" s="92"/>
-      <c r="H40" s="92"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="92"/>
-      <c r="K40" s="92"/>
-      <c r="L40" s="92"/>
-      <c r="M40" s="92"/>
-      <c r="N40" s="92"/>
-      <c r="O40" s="93"/>
+      <c r="E40" s="108"/>
+      <c r="F40" s="108"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="108"/>
+      <c r="I40" s="108"/>
+      <c r="J40" s="108"/>
+      <c r="K40" s="108"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="108"/>
+      <c r="N40" s="108"/>
+      <c r="O40" s="109"/>
       <c r="P40" s="86"/>
       <c r="Q40" s="86"/>
       <c r="R40" s="86"/>
@@ -21995,20 +22037,20 @@
       <c r="C41" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D41" s="91" t="s">
+      <c r="D41" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="92"/>
-      <c r="F41" s="92"/>
-      <c r="G41" s="92"/>
-      <c r="H41" s="92"/>
-      <c r="I41" s="92"/>
-      <c r="J41" s="92"/>
-      <c r="K41" s="92"/>
-      <c r="L41" s="92"/>
-      <c r="M41" s="92"/>
-      <c r="N41" s="92"/>
-      <c r="O41" s="93"/>
+      <c r="E41" s="108"/>
+      <c r="F41" s="108"/>
+      <c r="G41" s="108"/>
+      <c r="H41" s="108"/>
+      <c r="I41" s="108"/>
+      <c r="J41" s="108"/>
+      <c r="K41" s="108"/>
+      <c r="L41" s="108"/>
+      <c r="M41" s="108"/>
+      <c r="N41" s="108"/>
+      <c r="O41" s="109"/>
       <c r="P41" s="86"/>
       <c r="Q41" s="86"/>
       <c r="R41" s="86"/>
@@ -22031,20 +22073,20 @@
       <c r="C42" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="D42" s="91" t="s">
+      <c r="D42" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E42" s="92"/>
-      <c r="F42" s="92"/>
-      <c r="G42" s="92"/>
-      <c r="H42" s="92"/>
-      <c r="I42" s="92"/>
-      <c r="J42" s="92"/>
-      <c r="K42" s="92"/>
-      <c r="L42" s="92"/>
-      <c r="M42" s="92"/>
-      <c r="N42" s="92"/>
-      <c r="O42" s="93"/>
+      <c r="E42" s="108"/>
+      <c r="F42" s="108"/>
+      <c r="G42" s="108"/>
+      <c r="H42" s="108"/>
+      <c r="I42" s="108"/>
+      <c r="J42" s="108"/>
+      <c r="K42" s="108"/>
+      <c r="L42" s="108"/>
+      <c r="M42" s="108"/>
+      <c r="N42" s="108"/>
+      <c r="O42" s="109"/>
       <c r="P42" s="86"/>
       <c r="Q42" s="86"/>
       <c r="R42" s="86"/>
@@ -22065,20 +22107,20 @@
         <v>222</v>
       </c>
       <c r="C43" s="56"/>
-      <c r="D43" s="91" t="s">
+      <c r="D43" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="E43" s="92"/>
-      <c r="F43" s="92"/>
-      <c r="G43" s="92"/>
-      <c r="H43" s="92"/>
-      <c r="I43" s="92"/>
-      <c r="J43" s="92"/>
-      <c r="K43" s="92"/>
-      <c r="L43" s="92"/>
-      <c r="M43" s="92"/>
-      <c r="N43" s="92"/>
-      <c r="O43" s="93"/>
+      <c r="E43" s="108"/>
+      <c r="F43" s="108"/>
+      <c r="G43" s="108"/>
+      <c r="H43" s="108"/>
+      <c r="I43" s="108"/>
+      <c r="J43" s="108"/>
+      <c r="K43" s="108"/>
+      <c r="L43" s="108"/>
+      <c r="M43" s="108"/>
+      <c r="N43" s="108"/>
+      <c r="O43" s="109"/>
       <c r="P43" s="86"/>
       <c r="Q43" s="86"/>
       <c r="R43" s="86"/>
@@ -22101,20 +22143,20 @@
       <c r="C44" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D44" s="91" t="s">
+      <c r="D44" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E44" s="92"/>
-      <c r="F44" s="92"/>
-      <c r="G44" s="92"/>
-      <c r="H44" s="92"/>
-      <c r="I44" s="92"/>
-      <c r="J44" s="92"/>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92"/>
-      <c r="M44" s="92"/>
-      <c r="N44" s="92"/>
-      <c r="O44" s="93"/>
+      <c r="E44" s="108"/>
+      <c r="F44" s="108"/>
+      <c r="G44" s="108"/>
+      <c r="H44" s="108"/>
+      <c r="I44" s="108"/>
+      <c r="J44" s="108"/>
+      <c r="K44" s="108"/>
+      <c r="L44" s="108"/>
+      <c r="M44" s="108"/>
+      <c r="N44" s="108"/>
+      <c r="O44" s="109"/>
       <c r="P44" s="86"/>
       <c r="Q44" s="86"/>
       <c r="R44" s="86"/>
@@ -22137,20 +22179,20 @@
       <c r="C45" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D45" s="91" t="s">
+      <c r="D45" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E45" s="92"/>
-      <c r="F45" s="92"/>
-      <c r="G45" s="92"/>
-      <c r="H45" s="92"/>
-      <c r="I45" s="92"/>
-      <c r="J45" s="92"/>
-      <c r="K45" s="92"/>
-      <c r="L45" s="92"/>
-      <c r="M45" s="92"/>
-      <c r="N45" s="92"/>
-      <c r="O45" s="93"/>
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="108"/>
+      <c r="I45" s="108"/>
+      <c r="J45" s="108"/>
+      <c r="K45" s="108"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="108"/>
+      <c r="N45" s="108"/>
+      <c r="O45" s="109"/>
       <c r="P45" s="86"/>
       <c r="Q45" s="86"/>
       <c r="R45" s="86"/>
@@ -22173,20 +22215,20 @@
       <c r="C46" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="D46" s="91" t="s">
+      <c r="D46" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E46" s="92"/>
-      <c r="F46" s="92"/>
-      <c r="G46" s="92"/>
-      <c r="H46" s="92"/>
-      <c r="I46" s="92"/>
-      <c r="J46" s="92"/>
-      <c r="K46" s="92"/>
-      <c r="L46" s="92"/>
-      <c r="M46" s="92"/>
-      <c r="N46" s="92"/>
-      <c r="O46" s="93"/>
+      <c r="E46" s="108"/>
+      <c r="F46" s="108"/>
+      <c r="G46" s="108"/>
+      <c r="H46" s="108"/>
+      <c r="I46" s="108"/>
+      <c r="J46" s="108"/>
+      <c r="K46" s="108"/>
+      <c r="L46" s="108"/>
+      <c r="M46" s="108"/>
+      <c r="N46" s="108"/>
+      <c r="O46" s="109"/>
       <c r="P46" s="86"/>
       <c r="Q46" s="86"/>
       <c r="R46" s="86"/>
@@ -22207,20 +22249,20 @@
         <v>223</v>
       </c>
       <c r="C47" s="56"/>
-      <c r="D47" s="91" t="s">
+      <c r="D47" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="92"/>
-      <c r="F47" s="92"/>
-      <c r="G47" s="92"/>
-      <c r="H47" s="92"/>
-      <c r="I47" s="92"/>
-      <c r="J47" s="92"/>
-      <c r="K47" s="92"/>
-      <c r="L47" s="92"/>
-      <c r="M47" s="92"/>
-      <c r="N47" s="92"/>
-      <c r="O47" s="93"/>
+      <c r="E47" s="108"/>
+      <c r="F47" s="108"/>
+      <c r="G47" s="108"/>
+      <c r="H47" s="108"/>
+      <c r="I47" s="108"/>
+      <c r="J47" s="108"/>
+      <c r="K47" s="108"/>
+      <c r="L47" s="108"/>
+      <c r="M47" s="108"/>
+      <c r="N47" s="108"/>
+      <c r="O47" s="109"/>
       <c r="P47" s="86"/>
       <c r="Q47" s="86"/>
       <c r="R47" s="86"/>
@@ -22243,20 +22285,20 @@
       <c r="C48" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D48" s="91" t="s">
+      <c r="D48" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="92"/>
-      <c r="F48" s="92"/>
-      <c r="G48" s="92"/>
-      <c r="H48" s="92"/>
-      <c r="I48" s="92"/>
-      <c r="J48" s="92"/>
-      <c r="K48" s="92"/>
-      <c r="L48" s="92"/>
-      <c r="M48" s="92"/>
-      <c r="N48" s="92"/>
-      <c r="O48" s="93"/>
+      <c r="E48" s="108"/>
+      <c r="F48" s="108"/>
+      <c r="G48" s="108"/>
+      <c r="H48" s="108"/>
+      <c r="I48" s="108"/>
+      <c r="J48" s="108"/>
+      <c r="K48" s="108"/>
+      <c r="L48" s="108"/>
+      <c r="M48" s="108"/>
+      <c r="N48" s="108"/>
+      <c r="O48" s="109"/>
       <c r="P48" s="86"/>
       <c r="Q48" s="86"/>
       <c r="R48" s="86"/>
@@ -22279,20 +22321,20 @@
       <c r="C49" s="57" t="s">
         <v>127</v>
       </c>
-      <c r="D49" s="91" t="s">
+      <c r="D49" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E49" s="92"/>
-      <c r="F49" s="92"/>
-      <c r="G49" s="92"/>
-      <c r="H49" s="92"/>
-      <c r="I49" s="92"/>
-      <c r="J49" s="92"/>
-      <c r="K49" s="92"/>
-      <c r="L49" s="92"/>
-      <c r="M49" s="92"/>
-      <c r="N49" s="92"/>
-      <c r="O49" s="93"/>
+      <c r="E49" s="108"/>
+      <c r="F49" s="108"/>
+      <c r="G49" s="108"/>
+      <c r="H49" s="108"/>
+      <c r="I49" s="108"/>
+      <c r="J49" s="108"/>
+      <c r="K49" s="108"/>
+      <c r="L49" s="108"/>
+      <c r="M49" s="108"/>
+      <c r="N49" s="108"/>
+      <c r="O49" s="109"/>
       <c r="P49" s="86"/>
       <c r="Q49" s="86"/>
       <c r="R49" s="86"/>
@@ -22315,20 +22357,20 @@
       <c r="C50" s="57" t="s">
         <v>126</v>
       </c>
-      <c r="D50" s="91" t="s">
+      <c r="D50" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="92"/>
-      <c r="F50" s="92"/>
-      <c r="G50" s="92"/>
-      <c r="H50" s="92"/>
-      <c r="I50" s="92"/>
-      <c r="J50" s="92"/>
-      <c r="K50" s="92"/>
-      <c r="L50" s="92"/>
-      <c r="M50" s="92"/>
-      <c r="N50" s="92"/>
-      <c r="O50" s="93"/>
+      <c r="E50" s="108"/>
+      <c r="F50" s="108"/>
+      <c r="G50" s="108"/>
+      <c r="H50" s="108"/>
+      <c r="I50" s="108"/>
+      <c r="J50" s="108"/>
+      <c r="K50" s="108"/>
+      <c r="L50" s="108"/>
+      <c r="M50" s="108"/>
+      <c r="N50" s="108"/>
+      <c r="O50" s="109"/>
       <c r="P50" s="86"/>
       <c r="Q50" s="86"/>
       <c r="R50" s="86"/>
@@ -22347,18 +22389,18 @@
       </c>
       <c r="B51" s="60"/>
       <c r="C51" s="61"/>
-      <c r="D51" s="94"/>
-      <c r="E51" s="95"/>
-      <c r="F51" s="95"/>
-      <c r="G51" s="95"/>
-      <c r="H51" s="95"/>
-      <c r="I51" s="95"/>
-      <c r="J51" s="95"/>
-      <c r="K51" s="95"/>
-      <c r="L51" s="95"/>
-      <c r="M51" s="95"/>
-      <c r="N51" s="95"/>
-      <c r="O51" s="96"/>
+      <c r="D51" s="124"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="125"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="125"/>
+      <c r="I51" s="125"/>
+      <c r="J51" s="125"/>
+      <c r="K51" s="125"/>
+      <c r="L51" s="125"/>
+      <c r="M51" s="125"/>
+      <c r="N51" s="125"/>
+      <c r="O51" s="126"/>
       <c r="P51" s="87"/>
       <c r="Q51" s="87"/>
       <c r="R51" s="87"/>
@@ -22379,20 +22421,20 @@
         <v>324</v>
       </c>
       <c r="C52" s="60"/>
-      <c r="D52" s="97" t="s">
+      <c r="D52" s="127" t="s">
         <v>95</v>
       </c>
-      <c r="E52" s="98"/>
-      <c r="F52" s="98"/>
-      <c r="G52" s="98"/>
-      <c r="H52" s="98"/>
-      <c r="I52" s="98"/>
-      <c r="J52" s="98"/>
-      <c r="K52" s="98"/>
-      <c r="L52" s="98"/>
-      <c r="M52" s="98"/>
-      <c r="N52" s="98"/>
-      <c r="O52" s="99"/>
+      <c r="E52" s="128"/>
+      <c r="F52" s="128"/>
+      <c r="G52" s="128"/>
+      <c r="H52" s="128"/>
+      <c r="I52" s="128"/>
+      <c r="J52" s="128"/>
+      <c r="K52" s="128"/>
+      <c r="L52" s="128"/>
+      <c r="M52" s="128"/>
+      <c r="N52" s="128"/>
+      <c r="O52" s="129"/>
       <c r="P52" s="87"/>
       <c r="Q52" s="87"/>
       <c r="R52" s="87"/>
@@ -22411,18 +22453,18 @@
       </c>
       <c r="B53" s="40"/>
       <c r="C53" s="2"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="101"/>
-      <c r="F53" s="101"/>
-      <c r="G53" s="101"/>
-      <c r="H53" s="101"/>
-      <c r="I53" s="101"/>
-      <c r="J53" s="101"/>
-      <c r="K53" s="101"/>
-      <c r="L53" s="101"/>
-      <c r="M53" s="101"/>
-      <c r="N53" s="101"/>
-      <c r="O53" s="101"/>
+      <c r="D53" s="130"/>
+      <c r="E53" s="131"/>
+      <c r="F53" s="131"/>
+      <c r="G53" s="131"/>
+      <c r="H53" s="131"/>
+      <c r="I53" s="131"/>
+      <c r="J53" s="131"/>
+      <c r="K53" s="131"/>
+      <c r="L53" s="131"/>
+      <c r="M53" s="131"/>
+      <c r="N53" s="131"/>
+      <c r="O53" s="131"/>
       <c r="P53" s="83"/>
       <c r="Q53" s="83"/>
       <c r="R53" s="83"/>
@@ -22443,20 +22485,20 @@
         <v>372</v>
       </c>
       <c r="C54" s="43"/>
-      <c r="D54" s="89" t="s">
+      <c r="D54" s="122" t="s">
         <v>347</v>
       </c>
-      <c r="E54" s="90"/>
-      <c r="F54" s="90"/>
-      <c r="G54" s="90"/>
-      <c r="H54" s="90"/>
-      <c r="I54" s="90"/>
-      <c r="J54" s="90"/>
-      <c r="K54" s="90"/>
-      <c r="L54" s="90"/>
-      <c r="M54" s="90"/>
-      <c r="N54" s="90"/>
-      <c r="O54" s="90"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="123"/>
+      <c r="G54" s="123"/>
+      <c r="H54" s="123"/>
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
+      <c r="K54" s="123"/>
+      <c r="L54" s="123"/>
+      <c r="M54" s="123"/>
+      <c r="N54" s="123"/>
+      <c r="O54" s="123"/>
       <c r="P54" s="83"/>
       <c r="Q54" s="83"/>
       <c r="R54" s="83"/>
@@ -22477,20 +22519,20 @@
         <v>373</v>
       </c>
       <c r="C55" s="43"/>
-      <c r="D55" s="89" t="s">
+      <c r="D55" s="122" t="s">
         <v>348</v>
       </c>
-      <c r="E55" s="90"/>
-      <c r="F55" s="90"/>
-      <c r="G55" s="90"/>
-      <c r="H55" s="90"/>
-      <c r="I55" s="90"/>
-      <c r="J55" s="90"/>
-      <c r="K55" s="90"/>
-      <c r="L55" s="90"/>
-      <c r="M55" s="90"/>
-      <c r="N55" s="90"/>
-      <c r="O55" s="90"/>
+      <c r="E55" s="123"/>
+      <c r="F55" s="123"/>
+      <c r="G55" s="123"/>
+      <c r="H55" s="123"/>
+      <c r="I55" s="123"/>
+      <c r="J55" s="123"/>
+      <c r="K55" s="123"/>
+      <c r="L55" s="123"/>
+      <c r="M55" s="123"/>
+      <c r="N55" s="123"/>
+      <c r="O55" s="123"/>
       <c r="P55" s="83" t="s">
         <v>374</v>
       </c>
@@ -23830,10 +23872,10 @@
         <v>360</v>
       </c>
       <c r="B103" s="49">
-        <v>3312</v>
+        <v>3311</v>
       </c>
       <c r="C103" s="49">
-        <v>2469</v>
+        <v>2470</v>
       </c>
       <c r="D103" s="49">
         <v>3044</v>
@@ -23854,13 +23896,13 @@
         <v>361</v>
       </c>
       <c r="B104" s="49">
-        <v>1101</v>
+        <v>1102</v>
       </c>
       <c r="C104" s="49">
-        <v>1329</v>
+        <v>1330</v>
       </c>
       <c r="D104" s="49">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="E104" s="49"/>
       <c r="F104" s="49"/>
@@ -23873,62 +23915,608 @@
       <c r="M104" s="49"/>
       <c r="N104" s="49"/>
     </row>
-    <row r="105" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105" s="42" t="s">
+        <v>375</v>
+      </c>
+      <c r="B105" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C105" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D105" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="106" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B106" s="42">
+        <v>3693</v>
+      </c>
+      <c r="C106" s="42">
+        <v>2828</v>
+      </c>
+      <c r="D106" s="42">
+        <v>3420</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B107" s="42">
+        <v>645</v>
+      </c>
+      <c r="C107" s="42">
+        <v>884</v>
+      </c>
+      <c r="D107" s="42">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="42" t="s">
+        <v>376</v>
+      </c>
+      <c r="B108" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C108" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D108" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A109" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B109" s="42">
+        <v>2709</v>
+      </c>
+      <c r="C109" s="42">
+        <v>2014</v>
+      </c>
+      <c r="D109" s="42">
+        <v>2554</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B110" s="42">
+        <v>925</v>
+      </c>
+      <c r="C110" s="42">
+        <v>1114</v>
+      </c>
+      <c r="D110" s="42">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="42" t="s">
+        <v>377</v>
+      </c>
+      <c r="B111" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C111" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D111" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B112" s="42">
+        <v>3813</v>
+      </c>
+      <c r="C112" s="42">
+        <v>2914</v>
+      </c>
+      <c r="D112" s="42">
+        <v>3530</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A113" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B113" s="42">
+        <v>598</v>
+      </c>
+      <c r="C113" s="42">
+        <v>859</v>
+      </c>
+      <c r="D113" s="42">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A114" s="42" t="s">
+        <v>378</v>
+      </c>
+      <c r="B114" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C114" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D114" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B115" s="42">
+        <v>3341</v>
+      </c>
+      <c r="C115" s="42">
+        <v>2520</v>
+      </c>
+      <c r="D115" s="42">
+        <v>3080</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A116" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B116" s="42">
+        <v>1098</v>
+      </c>
+      <c r="C116" s="42">
+        <v>1349</v>
+      </c>
+      <c r="D116" s="42">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A117" s="42" t="s">
+        <v>379</v>
+      </c>
+      <c r="B117" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C117" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D117" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A118" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B118" s="42">
+        <v>4133</v>
+      </c>
+      <c r="C118" s="42">
+        <v>3142</v>
+      </c>
+      <c r="D118" s="42">
+        <v>3818</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B119" s="42">
+        <v>1105</v>
+      </c>
+      <c r="C119" s="42">
+        <v>1377</v>
+      </c>
+      <c r="D119" s="42">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A120" s="42" t="s">
+        <v>380</v>
+      </c>
+      <c r="B120" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C120" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D120" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A121" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B121" s="42">
+        <v>3472</v>
+      </c>
+      <c r="C121" s="42">
+        <v>2645</v>
+      </c>
+      <c r="D121" s="42">
+        <v>3208</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A122" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B122" s="42">
+        <v>796</v>
+      </c>
+      <c r="C122" s="42">
+        <v>1032</v>
+      </c>
+      <c r="D122" s="42">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A123" s="42" t="s">
+        <v>381</v>
+      </c>
+      <c r="B123" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C123" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D123" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B124" s="42">
+        <v>3325</v>
+      </c>
+      <c r="C124" s="42">
+        <v>2524</v>
+      </c>
+      <c r="D124" s="42">
+        <v>3069</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A125" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B125" s="42">
+        <v>871</v>
+      </c>
+      <c r="C125" s="42">
+        <v>1101</v>
+      </c>
+      <c r="D125" s="42">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A126" s="42" t="s">
+        <v>382</v>
+      </c>
+      <c r="B126" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C126" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D126" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A127" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B127" s="42">
+        <v>3209</v>
+      </c>
+      <c r="C127" s="42">
+        <v>2437</v>
+      </c>
+      <c r="D127" s="42">
+        <v>2966</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A128" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B128" s="42">
+        <v>703</v>
+      </c>
+      <c r="C128" s="42">
+        <v>916</v>
+      </c>
+      <c r="D128" s="42">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A129" s="42" t="s">
+        <v>383</v>
+      </c>
+      <c r="B129" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C129" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D129" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A130" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B130" s="42">
+        <v>2947</v>
+      </c>
+      <c r="C130" s="42">
+        <v>2200</v>
+      </c>
+      <c r="D130" s="42">
+        <v>2711</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A131" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B131" s="42">
+        <v>797</v>
+      </c>
+      <c r="C131" s="42">
+        <v>995</v>
+      </c>
+      <c r="D131" s="42">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A132" s="42" t="s">
+        <v>384</v>
+      </c>
+      <c r="B132" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C132" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D132" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B133" s="42">
+        <v>3727</v>
+      </c>
+      <c r="C133" s="42">
+        <v>2884</v>
+      </c>
+      <c r="D133" s="42">
+        <v>3457</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A134" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B134" s="42">
+        <v>1346</v>
+      </c>
+      <c r="C134" s="42">
+        <v>1589</v>
+      </c>
+      <c r="D134" s="42">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A135" s="42" t="s">
+        <v>385</v>
+      </c>
+      <c r="B135" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C135" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D135" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B136" s="42">
+        <v>3297</v>
+      </c>
+      <c r="C136" s="42">
+        <v>2473</v>
+      </c>
+      <c r="D136" s="42">
+        <v>3038</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A137" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B137" s="42">
+        <v>1237</v>
+      </c>
+      <c r="C137" s="42">
+        <v>1456</v>
+      </c>
+      <c r="D137" s="42">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="42" t="s">
+        <v>386</v>
+      </c>
+      <c r="B138" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C138" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D138" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B139" s="42">
+        <v>3280</v>
+      </c>
+      <c r="C139" s="42">
+        <v>2511</v>
+      </c>
+      <c r="D139" s="42">
+        <v>3035</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A140" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B140" s="42">
+        <v>1110</v>
+      </c>
+      <c r="C140" s="42">
+        <v>1341</v>
+      </c>
+      <c r="D140" s="42">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A141" s="42" t="s">
+        <v>387</v>
+      </c>
+      <c r="B141" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C141" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D141" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A142" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B142" s="42">
+        <v>3551</v>
+      </c>
+      <c r="C142" s="42">
+        <v>2703</v>
+      </c>
+      <c r="D142" s="42">
+        <v>3280</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B143" s="42">
+        <v>1167</v>
+      </c>
+      <c r="C143" s="42">
+        <v>1402</v>
+      </c>
+      <c r="D143" s="42">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="42" t="s">
+        <v>388</v>
+      </c>
+      <c r="B144" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="C144" s="42" t="s">
+        <v>359</v>
+      </c>
+      <c r="D144" s="42" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B145" s="42">
+        <v>3246</v>
+      </c>
+      <c r="C145" s="42">
+        <v>2449</v>
+      </c>
+      <c r="D145" s="42">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A146" s="42" t="s">
+        <v>361</v>
+      </c>
+      <c r="B146" s="42">
+        <v>1134</v>
+      </c>
+      <c r="C146" s="42">
+        <v>1358</v>
+      </c>
+      <c r="D146" s="42">
+        <v>1173</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -24764,6 +25352,49 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="D55:O55"/>
+    <mergeCell ref="D49:O49"/>
+    <mergeCell ref="D50:O50"/>
+    <mergeCell ref="D51:O51"/>
+    <mergeCell ref="D52:O52"/>
+    <mergeCell ref="D53:O53"/>
+    <mergeCell ref="D54:O54"/>
+    <mergeCell ref="D48:O48"/>
+    <mergeCell ref="D37:O37"/>
+    <mergeCell ref="D38:O38"/>
+    <mergeCell ref="D39:O39"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D41:O41"/>
+    <mergeCell ref="D42:O42"/>
+    <mergeCell ref="D43:O43"/>
+    <mergeCell ref="D44:O44"/>
+    <mergeCell ref="D45:O45"/>
+    <mergeCell ref="D46:O46"/>
+    <mergeCell ref="D47:O47"/>
+    <mergeCell ref="D36:O36"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D26:O26"/>
+    <mergeCell ref="D27:O27"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="D29:O29"/>
+    <mergeCell ref="D30:O30"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="D33:O33"/>
+    <mergeCell ref="D34:O34"/>
+    <mergeCell ref="D35:O35"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="D14:O14"/>
+    <mergeCell ref="D15:O15"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="D17:O17"/>
+    <mergeCell ref="D18:O18"/>
+    <mergeCell ref="D19:O19"/>
+    <mergeCell ref="D20:O20"/>
+    <mergeCell ref="D21:O21"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D23:O23"/>
     <mergeCell ref="D12:O12"/>
     <mergeCell ref="D1:O1"/>
     <mergeCell ref="D2:O2"/>
@@ -24776,49 +25407,6 @@
     <mergeCell ref="D9:O9"/>
     <mergeCell ref="D10:O10"/>
     <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="D14:O14"/>
-    <mergeCell ref="D15:O15"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="D17:O17"/>
-    <mergeCell ref="D18:O18"/>
-    <mergeCell ref="D19:O19"/>
-    <mergeCell ref="D20:O20"/>
-    <mergeCell ref="D21:O21"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D36:O36"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D26:O26"/>
-    <mergeCell ref="D27:O27"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="D29:O29"/>
-    <mergeCell ref="D30:O30"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="D32:O32"/>
-    <mergeCell ref="D33:O33"/>
-    <mergeCell ref="D34:O34"/>
-    <mergeCell ref="D35:O35"/>
-    <mergeCell ref="D48:O48"/>
-    <mergeCell ref="D37:O37"/>
-    <mergeCell ref="D38:O38"/>
-    <mergeCell ref="D39:O39"/>
-    <mergeCell ref="D40:O40"/>
-    <mergeCell ref="D41:O41"/>
-    <mergeCell ref="D42:O42"/>
-    <mergeCell ref="D43:O43"/>
-    <mergeCell ref="D44:O44"/>
-    <mergeCell ref="D45:O45"/>
-    <mergeCell ref="D46:O46"/>
-    <mergeCell ref="D47:O47"/>
-    <mergeCell ref="D55:O55"/>
-    <mergeCell ref="D49:O49"/>
-    <mergeCell ref="D50:O50"/>
-    <mergeCell ref="D51:O51"/>
-    <mergeCell ref="D52:O52"/>
-    <mergeCell ref="D53:O53"/>
-    <mergeCell ref="D54:O54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
no more package, active/inactive possibility
</commit_message>
<xml_diff>
--- a/Database/CoastSnapPyDB.xlsx
+++ b/Database/CoastSnapPyDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathvansoest/Documents/CoastSnapPy/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8986F73-5211-634D-9E83-920C36324CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8DCDEC4-3B04-9140-8D32-D2DBCA9773F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="egmond" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="137">
   <si>
     <t>Station Data</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>target22.jpg</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>INACTIVE</t>
   </si>
 </sst>
 </file>
@@ -443,7 +449,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -719,20 +725,50 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -745,36 +781,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1091,8 +1097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82C2A5-FA5F-4BBC-B066-D9DA22911E90}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="B130" sqref="B130:D131"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1109,20 +1115,22 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="C1" s="10"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="81"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="47"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -1143,20 +1151,20 @@
       <c r="C2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="84"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="50"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1177,20 +1185,20 @@
       <c r="C3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="84"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="49"/>
+      <c r="O3" s="50"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -1211,20 +1219,20 @@
       <c r="C4" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="84"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
+      <c r="K4" s="49"/>
+      <c r="L4" s="49"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="49"/>
+      <c r="O4" s="50"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -1243,20 +1251,20 @@
         <v>73</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="48" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="84"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
+      <c r="M5" s="49"/>
+      <c r="N5" s="49"/>
+      <c r="O5" s="50"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -1277,20 +1285,20 @@
       <c r="C6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="84"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="50"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -1311,20 +1319,20 @@
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="84"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="49"/>
+      <c r="L7" s="49"/>
+      <c r="M7" s="49"/>
+      <c r="N7" s="49"/>
+      <c r="O7" s="50"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -1345,20 +1353,20 @@
       <c r="C8" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="84"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="M8" s="49"/>
+      <c r="N8" s="49"/>
+      <c r="O8" s="50"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1379,20 +1387,20 @@
       <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="84"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
+      <c r="M9" s="49"/>
+      <c r="N9" s="49"/>
+      <c r="O9" s="50"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1409,18 +1417,18 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="75"/>
+      <c r="D10" s="51"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="53"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
@@ -1441,20 +1449,20 @@
       <c r="C11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="42" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="72"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="44"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
@@ -1475,20 +1483,20 @@
       <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="42" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="72"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="44"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
@@ -1509,20 +1517,20 @@
       <c r="C13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="72"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="44"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
@@ -1543,20 +1551,20 @@
       <c r="C14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="71"/>
-      <c r="O14" s="72"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="44"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
@@ -1577,20 +1585,20 @@
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="71"/>
-      <c r="O15" s="72"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="44"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
@@ -1611,20 +1619,20 @@
       <c r="C16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="71"/>
-      <c r="N16" s="71"/>
-      <c r="O16" s="72"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="44"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
@@ -1645,20 +1653,20 @@
       <c r="C17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="72"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="44"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
@@ -1679,20 +1687,20 @@
       <c r="C18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="70" t="s">
+      <c r="D18" s="42" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="71"/>
-      <c r="N18" s="71"/>
-      <c r="O18" s="72"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="43"/>
+      <c r="O18" s="44"/>
       <c r="P18" s="35"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
@@ -1715,20 +1723,20 @@
       <c r="C19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="51" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="74"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="75"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
       <c r="P19" s="35"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="35"/>
@@ -1751,20 +1759,20 @@
       <c r="C20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="75"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53"/>
       <c r="P20" s="35"/>
       <c r="Q20" s="35"/>
       <c r="R20" s="35"/>
@@ -1787,20 +1795,20 @@
       <c r="C21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="75"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="53"/>
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="35"/>
@@ -1823,20 +1831,20 @@
       <c r="C22" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="D22" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="72"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="44"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="35"/>
       <c r="R22" s="35"/>
@@ -1855,18 +1863,18 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="78"/>
+      <c r="D23" s="57"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="58"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="59"/>
       <c r="P23" s="37"/>
       <c r="Q23" s="37"/>
       <c r="R23" s="37"/>
@@ -1887,20 +1895,20 @@
         <v>81</v>
       </c>
       <c r="C24" s="19"/>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="E24" s="55"/>
+      <c r="F24" s="55"/>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
+      <c r="I24" s="55"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="56"/>
       <c r="P24" s="37"/>
       <c r="Q24" s="37"/>
       <c r="R24" s="37"/>
@@ -1923,20 +1931,20 @@
       <c r="C25" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="54" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="57"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
+      <c r="I25" s="55"/>
+      <c r="J25" s="55"/>
+      <c r="K25" s="55"/>
+      <c r="L25" s="55"/>
+      <c r="M25" s="55"/>
+      <c r="N25" s="55"/>
+      <c r="O25" s="56"/>
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
       <c r="R25" s="37"/>
@@ -1955,18 +1963,18 @@
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="60"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="64"/>
+      <c r="F26" s="64"/>
+      <c r="G26" s="64"/>
+      <c r="H26" s="64"/>
+      <c r="I26" s="64"/>
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="64"/>
+      <c r="N26" s="64"/>
+      <c r="O26" s="65"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="38"/>
       <c r="R26" s="38"/>
@@ -1987,20 +1995,20 @@
         <v>83</v>
       </c>
       <c r="C27" s="22"/>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="63"/>
+      <c r="E27" s="67"/>
+      <c r="F27" s="67"/>
+      <c r="G27" s="67"/>
+      <c r="H27" s="67"/>
+      <c r="I27" s="67"/>
+      <c r="J27" s="67"/>
+      <c r="K27" s="67"/>
+      <c r="L27" s="67"/>
+      <c r="M27" s="67"/>
+      <c r="N27" s="67"/>
+      <c r="O27" s="68"/>
       <c r="P27" s="38"/>
       <c r="Q27" s="38"/>
       <c r="R27" s="38"/>
@@ -2021,20 +2029,20 @@
         <v>32</v>
       </c>
       <c r="C28" s="22"/>
-      <c r="D28" s="64" t="s">
+      <c r="D28" s="69" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="66"/>
+      <c r="E28" s="70"/>
+      <c r="F28" s="70"/>
+      <c r="G28" s="70"/>
+      <c r="H28" s="70"/>
+      <c r="I28" s="70"/>
+      <c r="J28" s="70"/>
+      <c r="K28" s="70"/>
+      <c r="L28" s="70"/>
+      <c r="M28" s="70"/>
+      <c r="N28" s="70"/>
+      <c r="O28" s="71"/>
       <c r="P28" s="38"/>
       <c r="Q28" s="38"/>
       <c r="R28" s="38"/>
@@ -2055,20 +2063,20 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C29" s="22"/>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="65"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="66"/>
+      <c r="E29" s="70"/>
+      <c r="F29" s="70"/>
+      <c r="G29" s="70"/>
+      <c r="H29" s="70"/>
+      <c r="I29" s="70"/>
+      <c r="J29" s="70"/>
+      <c r="K29" s="70"/>
+      <c r="L29" s="70"/>
+      <c r="M29" s="70"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="71"/>
       <c r="P29" s="38"/>
       <c r="Q29" s="38"/>
       <c r="R29" s="38"/>
@@ -2087,20 +2095,20 @@
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="26"/>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
-      <c r="O30" s="69"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="73"/>
+      <c r="K30" s="73"/>
+      <c r="L30" s="73"/>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="74"/>
       <c r="P30" s="39"/>
       <c r="Q30" s="39"/>
       <c r="R30" s="39"/>
@@ -2121,20 +2129,20 @@
         <v>76</v>
       </c>
       <c r="C31" s="26"/>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="46"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="61"/>
+      <c r="L31" s="61"/>
+      <c r="M31" s="61"/>
+      <c r="N31" s="61"/>
+      <c r="O31" s="62"/>
       <c r="P31" s="39"/>
       <c r="Q31" s="39"/>
       <c r="R31" s="39"/>
@@ -2157,20 +2165,20 @@
       <c r="C32" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="46"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="62"/>
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
       <c r="R32" s="39"/>
@@ -2193,20 +2201,20 @@
       <c r="C33" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="46"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="62"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
       <c r="R33" s="39"/>
@@ -2229,20 +2237,20 @@
       <c r="C34" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="46"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="61"/>
+      <c r="L34" s="61"/>
+      <c r="M34" s="61"/>
+      <c r="N34" s="61"/>
+      <c r="O34" s="62"/>
       <c r="P34" s="39"/>
       <c r="Q34" s="39"/>
       <c r="R34" s="39"/>
@@ -2263,20 +2271,20 @@
         <v>77</v>
       </c>
       <c r="C35" s="26"/>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="46"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="61"/>
+      <c r="K35" s="61"/>
+      <c r="L35" s="61"/>
+      <c r="M35" s="61"/>
+      <c r="N35" s="61"/>
+      <c r="O35" s="62"/>
       <c r="P35" s="39"/>
       <c r="Q35" s="39"/>
       <c r="R35" s="39"/>
@@ -2299,20 +2307,20 @@
       <c r="C36" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="46"/>
+      <c r="E36" s="61"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="61"/>
+      <c r="I36" s="61"/>
+      <c r="J36" s="61"/>
+      <c r="K36" s="61"/>
+      <c r="L36" s="61"/>
+      <c r="M36" s="61"/>
+      <c r="N36" s="61"/>
+      <c r="O36" s="62"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
       <c r="R36" s="39"/>
@@ -2335,20 +2343,20 @@
       <c r="C37" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="44" t="s">
+      <c r="D37" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="46"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="61"/>
+      <c r="I37" s="61"/>
+      <c r="J37" s="61"/>
+      <c r="K37" s="61"/>
+      <c r="L37" s="61"/>
+      <c r="M37" s="61"/>
+      <c r="N37" s="61"/>
+      <c r="O37" s="62"/>
       <c r="P37" s="39"/>
       <c r="Q37" s="39"/>
       <c r="R37" s="39"/>
@@ -2371,20 +2379,20 @@
       <c r="C38" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="46"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="G38" s="61"/>
+      <c r="H38" s="61"/>
+      <c r="I38" s="61"/>
+      <c r="J38" s="61"/>
+      <c r="K38" s="61"/>
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="62"/>
       <c r="P38" s="39"/>
       <c r="Q38" s="39"/>
       <c r="R38" s="39"/>
@@ -2405,20 +2413,20 @@
         <v>78</v>
       </c>
       <c r="C39" s="25"/>
-      <c r="D39" s="44" t="s">
+      <c r="D39" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="46"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="61"/>
+      <c r="G39" s="61"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="61"/>
+      <c r="J39" s="61"/>
+      <c r="K39" s="61"/>
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="62"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
       <c r="R39" s="39"/>
@@ -2441,20 +2449,20 @@
       <c r="C40" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="46"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="61"/>
+      <c r="J40" s="61"/>
+      <c r="K40" s="61"/>
+      <c r="L40" s="61"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="61"/>
+      <c r="O40" s="62"/>
       <c r="P40" s="39"/>
       <c r="Q40" s="39"/>
       <c r="R40" s="39"/>
@@ -2477,20 +2485,20 @@
       <c r="C41" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="44" t="s">
+      <c r="D41" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="46"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="61"/>
+      <c r="K41" s="61"/>
+      <c r="L41" s="61"/>
+      <c r="M41" s="61"/>
+      <c r="N41" s="61"/>
+      <c r="O41" s="62"/>
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
       <c r="R41" s="39"/>
@@ -2513,20 +2521,20 @@
       <c r="C42" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="44" t="s">
+      <c r="D42" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="46"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="61"/>
+      <c r="K42" s="61"/>
+      <c r="L42" s="61"/>
+      <c r="M42" s="61"/>
+      <c r="N42" s="61"/>
+      <c r="O42" s="62"/>
       <c r="P42" s="39"/>
       <c r="Q42" s="39"/>
       <c r="R42" s="39"/>
@@ -2547,20 +2555,20 @@
         <v>79</v>
       </c>
       <c r="C43" s="25"/>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="46"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="61"/>
+      <c r="J43" s="61"/>
+      <c r="K43" s="61"/>
+      <c r="L43" s="61"/>
+      <c r="M43" s="61"/>
+      <c r="N43" s="61"/>
+      <c r="O43" s="62"/>
       <c r="P43" s="39"/>
       <c r="Q43" s="39"/>
       <c r="R43" s="39"/>
@@ -2583,20 +2591,20 @@
       <c r="C44" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="46"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="61"/>
+      <c r="J44" s="61"/>
+      <c r="K44" s="61"/>
+      <c r="L44" s="61"/>
+      <c r="M44" s="61"/>
+      <c r="N44" s="61"/>
+      <c r="O44" s="62"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="39"/>
       <c r="R44" s="39"/>
@@ -2619,20 +2627,20 @@
       <c r="C45" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="44" t="s">
+      <c r="D45" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="45"/>
-      <c r="O45" s="46"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="61"/>
+      <c r="J45" s="61"/>
+      <c r="K45" s="61"/>
+      <c r="L45" s="61"/>
+      <c r="M45" s="61"/>
+      <c r="N45" s="61"/>
+      <c r="O45" s="62"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
       <c r="R45" s="39"/>
@@ -2655,20 +2663,20 @@
       <c r="C46" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="46"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="61"/>
+      <c r="J46" s="61"/>
+      <c r="K46" s="61"/>
+      <c r="L46" s="61"/>
+      <c r="M46" s="61"/>
+      <c r="N46" s="61"/>
+      <c r="O46" s="62"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
       <c r="R46" s="39"/>
@@ -2689,20 +2697,20 @@
         <v>80</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="46"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="61"/>
+      <c r="I47" s="61"/>
+      <c r="J47" s="61"/>
+      <c r="K47" s="61"/>
+      <c r="L47" s="61"/>
+      <c r="M47" s="61"/>
+      <c r="N47" s="61"/>
+      <c r="O47" s="62"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="39"/>
       <c r="R47" s="39"/>
@@ -2725,20 +2733,20 @@
       <c r="C48" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="45"/>
-      <c r="N48" s="45"/>
-      <c r="O48" s="46"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="61"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="61"/>
+      <c r="I48" s="61"/>
+      <c r="J48" s="61"/>
+      <c r="K48" s="61"/>
+      <c r="L48" s="61"/>
+      <c r="M48" s="61"/>
+      <c r="N48" s="61"/>
+      <c r="O48" s="62"/>
       <c r="P48" s="39"/>
       <c r="Q48" s="39"/>
       <c r="R48" s="39"/>
@@ -2761,20 +2769,20 @@
       <c r="C49" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="44" t="s">
+      <c r="D49" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="46"/>
+      <c r="E49" s="61"/>
+      <c r="F49" s="61"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="61"/>
+      <c r="I49" s="61"/>
+      <c r="J49" s="61"/>
+      <c r="K49" s="61"/>
+      <c r="L49" s="61"/>
+      <c r="M49" s="61"/>
+      <c r="N49" s="61"/>
+      <c r="O49" s="62"/>
       <c r="P49" s="39"/>
       <c r="Q49" s="39"/>
       <c r="R49" s="39"/>
@@ -2797,20 +2805,20 @@
       <c r="C50" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="44" t="s">
+      <c r="D50" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="45"/>
-      <c r="M50" s="45"/>
-      <c r="N50" s="45"/>
-      <c r="O50" s="46"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="61"/>
+      <c r="I50" s="61"/>
+      <c r="J50" s="61"/>
+      <c r="K50" s="61"/>
+      <c r="L50" s="61"/>
+      <c r="M50" s="61"/>
+      <c r="N50" s="61"/>
+      <c r="O50" s="62"/>
       <c r="P50" s="39"/>
       <c r="Q50" s="39"/>
       <c r="R50" s="39"/>
@@ -2829,18 +2837,18 @@
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="30"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="49"/>
+      <c r="D51" s="77"/>
+      <c r="E51" s="78"/>
+      <c r="F51" s="78"/>
+      <c r="G51" s="78"/>
+      <c r="H51" s="78"/>
+      <c r="I51" s="78"/>
+      <c r="J51" s="78"/>
+      <c r="K51" s="78"/>
+      <c r="L51" s="78"/>
+      <c r="M51" s="78"/>
+      <c r="N51" s="78"/>
+      <c r="O51" s="79"/>
       <c r="P51" s="40"/>
       <c r="Q51" s="40"/>
       <c r="R51" s="40"/>
@@ -2861,20 +2869,20 @@
         <v>82</v>
       </c>
       <c r="C52" s="29"/>
-      <c r="D52" s="50" t="s">
+      <c r="D52" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="51"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="52"/>
+      <c r="E52" s="81"/>
+      <c r="F52" s="81"/>
+      <c r="G52" s="81"/>
+      <c r="H52" s="81"/>
+      <c r="I52" s="81"/>
+      <c r="J52" s="81"/>
+      <c r="K52" s="81"/>
+      <c r="L52" s="81"/>
+      <c r="M52" s="81"/>
+      <c r="N52" s="81"/>
+      <c r="O52" s="82"/>
       <c r="P52" s="40"/>
       <c r="Q52" s="40"/>
       <c r="R52" s="40"/>
@@ -2893,18 +2901,18 @@
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="54"/>
-      <c r="M53" s="54"/>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
+      <c r="D53" s="83"/>
+      <c r="E53" s="84"/>
+      <c r="F53" s="84"/>
+      <c r="G53" s="84"/>
+      <c r="H53" s="84"/>
+      <c r="I53" s="84"/>
+      <c r="J53" s="84"/>
+      <c r="K53" s="84"/>
+      <c r="L53" s="84"/>
+      <c r="M53" s="84"/>
+      <c r="N53" s="84"/>
+      <c r="O53" s="84"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="36"/>
       <c r="R53" s="36"/>
@@ -2925,20 +2933,20 @@
         <v>118</v>
       </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="42" t="s">
+      <c r="D54" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="43"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="43"/>
-      <c r="O54" s="43"/>
+      <c r="E54" s="76"/>
+      <c r="F54" s="76"/>
+      <c r="G54" s="76"/>
+      <c r="H54" s="76"/>
+      <c r="I54" s="76"/>
+      <c r="J54" s="76"/>
+      <c r="K54" s="76"/>
+      <c r="L54" s="76"/>
+      <c r="M54" s="76"/>
+      <c r="N54" s="76"/>
+      <c r="O54" s="76"/>
       <c r="P54" s="36"/>
       <c r="Q54" s="36"/>
       <c r="R54" s="36"/>
@@ -2959,20 +2967,20 @@
         <v>119</v>
       </c>
       <c r="C55" s="12"/>
-      <c r="D55" s="42" t="s">
+      <c r="D55" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="43"/>
+      <c r="E55" s="76"/>
+      <c r="F55" s="76"/>
+      <c r="G55" s="76"/>
+      <c r="H55" s="76"/>
+      <c r="I55" s="76"/>
+      <c r="J55" s="76"/>
+      <c r="K55" s="76"/>
+      <c r="L55" s="76"/>
+      <c r="M55" s="76"/>
+      <c r="N55" s="76"/>
+      <c r="O55" s="76"/>
       <c r="P55" s="36" t="s">
         <v>120</v>
       </c>
@@ -5792,6 +5800,49 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="D55:O55"/>
+    <mergeCell ref="D49:O49"/>
+    <mergeCell ref="D50:O50"/>
+    <mergeCell ref="D51:O51"/>
+    <mergeCell ref="D52:O52"/>
+    <mergeCell ref="D53:O53"/>
+    <mergeCell ref="D54:O54"/>
+    <mergeCell ref="D48:O48"/>
+    <mergeCell ref="D37:O37"/>
+    <mergeCell ref="D38:O38"/>
+    <mergeCell ref="D39:O39"/>
+    <mergeCell ref="D40:O40"/>
+    <mergeCell ref="D41:O41"/>
+    <mergeCell ref="D42:O42"/>
+    <mergeCell ref="D43:O43"/>
+    <mergeCell ref="D44:O44"/>
+    <mergeCell ref="D45:O45"/>
+    <mergeCell ref="D46:O46"/>
+    <mergeCell ref="D47:O47"/>
+    <mergeCell ref="D36:O36"/>
+    <mergeCell ref="D25:O25"/>
+    <mergeCell ref="D26:O26"/>
+    <mergeCell ref="D27:O27"/>
+    <mergeCell ref="D28:O28"/>
+    <mergeCell ref="D29:O29"/>
+    <mergeCell ref="D30:O30"/>
+    <mergeCell ref="D31:O31"/>
+    <mergeCell ref="D32:O32"/>
+    <mergeCell ref="D33:O33"/>
+    <mergeCell ref="D34:O34"/>
+    <mergeCell ref="D35:O35"/>
+    <mergeCell ref="D24:O24"/>
+    <mergeCell ref="D13:O13"/>
+    <mergeCell ref="D14:O14"/>
+    <mergeCell ref="D15:O15"/>
+    <mergeCell ref="D16:O16"/>
+    <mergeCell ref="D17:O17"/>
+    <mergeCell ref="D18:O18"/>
+    <mergeCell ref="D19:O19"/>
+    <mergeCell ref="D20:O20"/>
+    <mergeCell ref="D21:O21"/>
+    <mergeCell ref="D22:O22"/>
+    <mergeCell ref="D23:O23"/>
     <mergeCell ref="D12:O12"/>
     <mergeCell ref="D1:O1"/>
     <mergeCell ref="D2:O2"/>
@@ -5804,49 +5855,6 @@
     <mergeCell ref="D9:O9"/>
     <mergeCell ref="D10:O10"/>
     <mergeCell ref="D11:O11"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D13:O13"/>
-    <mergeCell ref="D14:O14"/>
-    <mergeCell ref="D15:O15"/>
-    <mergeCell ref="D16:O16"/>
-    <mergeCell ref="D17:O17"/>
-    <mergeCell ref="D18:O18"/>
-    <mergeCell ref="D19:O19"/>
-    <mergeCell ref="D20:O20"/>
-    <mergeCell ref="D21:O21"/>
-    <mergeCell ref="D22:O22"/>
-    <mergeCell ref="D23:O23"/>
-    <mergeCell ref="D36:O36"/>
-    <mergeCell ref="D25:O25"/>
-    <mergeCell ref="D26:O26"/>
-    <mergeCell ref="D27:O27"/>
-    <mergeCell ref="D28:O28"/>
-    <mergeCell ref="D29:O29"/>
-    <mergeCell ref="D30:O30"/>
-    <mergeCell ref="D31:O31"/>
-    <mergeCell ref="D32:O32"/>
-    <mergeCell ref="D33:O33"/>
-    <mergeCell ref="D34:O34"/>
-    <mergeCell ref="D35:O35"/>
-    <mergeCell ref="D48:O48"/>
-    <mergeCell ref="D37:O37"/>
-    <mergeCell ref="D38:O38"/>
-    <mergeCell ref="D39:O39"/>
-    <mergeCell ref="D40:O40"/>
-    <mergeCell ref="D41:O41"/>
-    <mergeCell ref="D42:O42"/>
-    <mergeCell ref="D43:O43"/>
-    <mergeCell ref="D44:O44"/>
-    <mergeCell ref="D45:O45"/>
-    <mergeCell ref="D46:O46"/>
-    <mergeCell ref="D47:O47"/>
-    <mergeCell ref="D55:O55"/>
-    <mergeCell ref="D49:O49"/>
-    <mergeCell ref="D50:O50"/>
-    <mergeCell ref="D51:O51"/>
-    <mergeCell ref="D52:O52"/>
-    <mergeCell ref="D53:O53"/>
-    <mergeCell ref="D54:O54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5857,8 +5865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD610E5-7CFE-40D9-832A-CDCE1C3A467E}">
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5874,7 +5882,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="C1" s="10"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>

</xml_diff>

<commit_message>
added sheets to DB.xlsx
</commit_message>
<xml_diff>
--- a/Database/CoastSnapPyDB.xlsx
+++ b/Database/CoastSnapPyDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathvansoest/Documents/CoastSnapPy/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E68227B2-118E-B44D-81E9-0FCA2D26C7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AABDC830-CB0D-FB4D-9D9F-3A029ECE179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="egmond" sheetId="10" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="135">
   <si>
     <t>Station Data</t>
   </si>
@@ -285,24 +285,9 @@
     <t>SLtransects_egmond.mat</t>
   </si>
   <si>
-    <t>HNK Paal</t>
-  </si>
-  <si>
-    <t>Reling Links</t>
-  </si>
-  <si>
-    <t>Reling Rechts</t>
-  </si>
-  <si>
-    <t>Houten Schot Rechts</t>
-  </si>
-  <si>
     <t>SLtransects_texel.mat</t>
   </si>
   <si>
-    <t>[1 2 3]</t>
-  </si>
-  <si>
     <t>Object Detection</t>
   </si>
   <si>
@@ -441,7 +426,16 @@
     <t>ACTIVE</t>
   </si>
   <si>
-    <t>INACTIVE</t>
+    <t>p5</t>
+  </si>
+  <si>
+    <t>HHNK</t>
+  </si>
+  <si>
+    <t>[1 2 3 4]</t>
+  </si>
+  <si>
+    <t>p6</t>
   </si>
 </sst>
 </file>
@@ -451,7 +445,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -539,6 +533,12 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -679,7 +679,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -734,6 +734,10 @@
     <xf numFmtId="0" fontId="13" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1097,8 +1101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82C2A5-FA5F-4BBC-B066-D9DA22911E90}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144:D146"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1116,21 +1120,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C1" s="10"/>
-      <c r="D1" s="79"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+      <c r="L1" s="82"/>
+      <c r="M1" s="82"/>
+      <c r="N1" s="82"/>
+      <c r="O1" s="83"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -1151,20 +1155,20 @@
       <c r="C2" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="82" t="s">
+      <c r="D2" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="84"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="86"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -1185,20 +1189,20 @@
       <c r="C3" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="84" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="84"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="86"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
@@ -1219,20 +1223,20 @@
       <c r="C4" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="82" t="s">
+      <c r="D4" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="83"/>
-      <c r="F4" s="83"/>
-      <c r="G4" s="83"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="83"/>
-      <c r="K4" s="83"/>
-      <c r="L4" s="83"/>
-      <c r="M4" s="83"/>
-      <c r="N4" s="83"/>
-      <c r="O4" s="84"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="85"/>
+      <c r="G4" s="85"/>
+      <c r="H4" s="85"/>
+      <c r="I4" s="85"/>
+      <c r="J4" s="85"/>
+      <c r="K4" s="85"/>
+      <c r="L4" s="85"/>
+      <c r="M4" s="85"/>
+      <c r="N4" s="85"/>
+      <c r="O4" s="86"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
@@ -1251,20 +1255,20 @@
         <v>73</v>
       </c>
       <c r="C5" s="12"/>
-      <c r="D5" s="82" t="s">
+      <c r="D5" s="84" t="s">
         <v>59</v>
       </c>
-      <c r="E5" s="83"/>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
-      <c r="N5" s="83"/>
-      <c r="O5" s="84"/>
+      <c r="E5" s="85"/>
+      <c r="F5" s="85"/>
+      <c r="G5" s="85"/>
+      <c r="H5" s="85"/>
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="86"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
@@ -1285,20 +1289,20 @@
       <c r="C6" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="82" t="s">
+      <c r="D6" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="83"/>
-      <c r="L6" s="83"/>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="84"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="85"/>
+      <c r="O6" s="86"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
@@ -1319,20 +1323,20 @@
       <c r="C7" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="82" t="s">
+      <c r="D7" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="83"/>
-      <c r="G7" s="83"/>
-      <c r="H7" s="83"/>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-      <c r="L7" s="83"/>
-      <c r="M7" s="83"/>
-      <c r="N7" s="83"/>
-      <c r="O7" s="84"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="85"/>
+      <c r="O7" s="86"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
@@ -1353,20 +1357,20 @@
       <c r="C8" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D8" s="82" t="s">
+      <c r="D8" s="84" t="s">
         <v>37</v>
       </c>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="84"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85"/>
+      <c r="I8" s="85"/>
+      <c r="J8" s="85"/>
+      <c r="K8" s="85"/>
+      <c r="L8" s="85"/>
+      <c r="M8" s="85"/>
+      <c r="N8" s="85"/>
+      <c r="O8" s="86"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
@@ -1387,20 +1391,20 @@
       <c r="C9" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="82" t="s">
+      <c r="D9" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="E9" s="83"/>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
-      <c r="N9" s="83"/>
-      <c r="O9" s="84"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="86"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
@@ -1417,18 +1421,18 @@
       </c>
       <c r="B10" s="15"/>
       <c r="C10" s="16"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="74"/>
-      <c r="L10" s="74"/>
-      <c r="M10" s="74"/>
-      <c r="N10" s="74"/>
-      <c r="O10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="76"/>
+      <c r="O10" s="77"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
@@ -1449,20 +1453,20 @@
       <c r="C11" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="71"/>
-      <c r="F11" s="71"/>
-      <c r="G11" s="71"/>
-      <c r="H11" s="71"/>
-      <c r="I11" s="71"/>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="71"/>
-      <c r="M11" s="71"/>
-      <c r="N11" s="71"/>
-      <c r="O11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73"/>
+      <c r="H11" s="73"/>
+      <c r="I11" s="73"/>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="73"/>
+      <c r="O11" s="74"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
@@ -1483,20 +1487,20 @@
       <c r="C12" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="71"/>
-      <c r="H12" s="71"/>
-      <c r="I12" s="71"/>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71"/>
-      <c r="L12" s="71"/>
-      <c r="M12" s="71"/>
-      <c r="N12" s="71"/>
-      <c r="O12" s="72"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
+      <c r="I12" s="73"/>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="73"/>
+      <c r="O12" s="74"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
@@ -1517,20 +1521,20 @@
       <c r="C13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D13" s="70" t="s">
+      <c r="D13" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="71"/>
-      <c r="F13" s="71"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71"/>
-      <c r="I13" s="71"/>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71"/>
-      <c r="L13" s="71"/>
-      <c r="M13" s="71"/>
-      <c r="N13" s="71"/>
-      <c r="O13" s="72"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="73"/>
+      <c r="J13" s="73"/>
+      <c r="K13" s="73"/>
+      <c r="L13" s="73"/>
+      <c r="M13" s="73"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="74"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
@@ -1551,20 +1555,20 @@
       <c r="C14" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="70" t="s">
+      <c r="D14" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="E14" s="71"/>
-      <c r="F14" s="71"/>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="71"/>
-      <c r="L14" s="71"/>
-      <c r="M14" s="71"/>
-      <c r="N14" s="71"/>
-      <c r="O14" s="72"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="73"/>
+      <c r="K14" s="73"/>
+      <c r="L14" s="73"/>
+      <c r="M14" s="73"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="74"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
@@ -1585,20 +1589,20 @@
       <c r="C15" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="71"/>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71"/>
-      <c r="I15" s="71"/>
-      <c r="J15" s="71"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="71"/>
-      <c r="M15" s="71"/>
-      <c r="N15" s="71"/>
-      <c r="O15" s="72"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="73"/>
+      <c r="K15" s="73"/>
+      <c r="L15" s="73"/>
+      <c r="M15" s="73"/>
+      <c r="N15" s="73"/>
+      <c r="O15" s="74"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
@@ -1619,20 +1623,20 @@
       <c r="C16" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="71"/>
-      <c r="J16" s="71"/>
-      <c r="K16" s="71"/>
-      <c r="L16" s="71"/>
-      <c r="M16" s="71"/>
-      <c r="N16" s="71"/>
-      <c r="O16" s="72"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="73"/>
+      <c r="K16" s="73"/>
+      <c r="L16" s="73"/>
+      <c r="M16" s="73"/>
+      <c r="N16" s="73"/>
+      <c r="O16" s="74"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
@@ -1653,20 +1657,20 @@
       <c r="C17" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="71"/>
-      <c r="F17" s="71"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71"/>
-      <c r="I17" s="71"/>
-      <c r="J17" s="71"/>
-      <c r="K17" s="71"/>
-      <c r="L17" s="71"/>
-      <c r="M17" s="71"/>
-      <c r="N17" s="71"/>
-      <c r="O17" s="72"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73"/>
+      <c r="H17" s="73"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="73"/>
+      <c r="K17" s="73"/>
+      <c r="L17" s="73"/>
+      <c r="M17" s="73"/>
+      <c r="N17" s="73"/>
+      <c r="O17" s="74"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="17"/>
       <c r="R17" s="17"/>
@@ -1687,20 +1691,20 @@
       <c r="C18" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="70" t="s">
+      <c r="D18" s="72" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="71"/>
-      <c r="F18" s="71"/>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="71"/>
-      <c r="M18" s="71"/>
-      <c r="N18" s="71"/>
-      <c r="O18" s="72"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="73"/>
+      <c r="K18" s="73"/>
+      <c r="L18" s="73"/>
+      <c r="M18" s="73"/>
+      <c r="N18" s="73"/>
+      <c r="O18" s="74"/>
       <c r="P18" s="35"/>
       <c r="Q18" s="35"/>
       <c r="R18" s="35"/>
@@ -1723,20 +1727,20 @@
       <c r="C19" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="75" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
-      <c r="I19" s="74"/>
-      <c r="J19" s="74"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="74"/>
-      <c r="M19" s="74"/>
-      <c r="N19" s="74"/>
-      <c r="O19" s="75"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="76"/>
+      <c r="J19" s="76"/>
+      <c r="K19" s="76"/>
+      <c r="L19" s="76"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="76"/>
+      <c r="O19" s="77"/>
       <c r="P19" s="35"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="35"/>
@@ -1759,20 +1763,20 @@
       <c r="C20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D20" s="73" t="s">
+      <c r="D20" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74"/>
-      <c r="H20" s="74"/>
-      <c r="I20" s="74"/>
-      <c r="J20" s="74"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="74"/>
-      <c r="M20" s="74"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="75"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="76"/>
+      <c r="K20" s="76"/>
+      <c r="L20" s="76"/>
+      <c r="M20" s="76"/>
+      <c r="N20" s="76"/>
+      <c r="O20" s="77"/>
       <c r="P20" s="35"/>
       <c r="Q20" s="35"/>
       <c r="R20" s="35"/>
@@ -1795,20 +1799,20 @@
       <c r="C21" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="75" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
-      <c r="I21" s="74"/>
-      <c r="J21" s="74"/>
-      <c r="K21" s="74"/>
-      <c r="L21" s="74"/>
-      <c r="M21" s="74"/>
-      <c r="N21" s="74"/>
-      <c r="O21" s="75"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="77"/>
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="35"/>
@@ -1831,20 +1835,20 @@
       <c r="C22" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="D22" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="E22" s="71"/>
-      <c r="F22" s="71"/>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="71"/>
-      <c r="L22" s="71"/>
-      <c r="M22" s="71"/>
-      <c r="N22" s="71"/>
-      <c r="O22" s="72"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
+      <c r="I22" s="73"/>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="73"/>
+      <c r="O22" s="74"/>
       <c r="P22" s="35"/>
       <c r="Q22" s="35"/>
       <c r="R22" s="35"/>
@@ -1863,18 +1867,18 @@
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="77"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="78"/>
+      <c r="D23" s="78"/>
+      <c r="E23" s="79"/>
+      <c r="F23" s="79"/>
+      <c r="G23" s="79"/>
+      <c r="H23" s="79"/>
+      <c r="I23" s="79"/>
+      <c r="J23" s="79"/>
+      <c r="K23" s="79"/>
+      <c r="L23" s="79"/>
+      <c r="M23" s="79"/>
+      <c r="N23" s="79"/>
+      <c r="O23" s="80"/>
       <c r="P23" s="37"/>
       <c r="Q23" s="37"/>
       <c r="R23" s="37"/>
@@ -1895,20 +1899,20 @@
         <v>81</v>
       </c>
       <c r="C24" s="19"/>
-      <c r="D24" s="55" t="s">
+      <c r="D24" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="56"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="56"/>
-      <c r="H24" s="56"/>
-      <c r="I24" s="56"/>
-      <c r="J24" s="56"/>
-      <c r="K24" s="56"/>
-      <c r="L24" s="56"/>
-      <c r="M24" s="56"/>
-      <c r="N24" s="56"/>
-      <c r="O24" s="57"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="58"/>
+      <c r="O24" s="59"/>
       <c r="P24" s="37"/>
       <c r="Q24" s="37"/>
       <c r="R24" s="37"/>
@@ -1931,20 +1935,20 @@
       <c r="C25" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="E25" s="56"/>
-      <c r="F25" s="56"/>
-      <c r="G25" s="56"/>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
-      <c r="L25" s="56"/>
-      <c r="M25" s="56"/>
-      <c r="N25" s="56"/>
-      <c r="O25" s="57"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="58"/>
+      <c r="I25" s="58"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="58"/>
+      <c r="L25" s="58"/>
+      <c r="M25" s="58"/>
+      <c r="N25" s="58"/>
+      <c r="O25" s="59"/>
       <c r="P25" s="37"/>
       <c r="Q25" s="37"/>
       <c r="R25" s="37"/>
@@ -1963,18 +1967,18 @@
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="59"/>
-      <c r="F26" s="59"/>
-      <c r="G26" s="59"/>
-      <c r="H26" s="59"/>
-      <c r="I26" s="59"/>
-      <c r="J26" s="59"/>
-      <c r="K26" s="59"/>
-      <c r="L26" s="59"/>
-      <c r="M26" s="59"/>
-      <c r="N26" s="59"/>
-      <c r="O26" s="60"/>
+      <c r="D26" s="60"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="62"/>
       <c r="P26" s="38"/>
       <c r="Q26" s="38"/>
       <c r="R26" s="38"/>
@@ -1995,20 +1999,20 @@
         <v>83</v>
       </c>
       <c r="C27" s="22"/>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="62"/>
-      <c r="K27" s="62"/>
-      <c r="L27" s="62"/>
-      <c r="M27" s="62"/>
-      <c r="N27" s="62"/>
-      <c r="O27" s="63"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
+      <c r="H27" s="64"/>
+      <c r="I27" s="64"/>
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="64"/>
+      <c r="N27" s="64"/>
+      <c r="O27" s="65"/>
       <c r="P27" s="38"/>
       <c r="Q27" s="38"/>
       <c r="R27" s="38"/>
@@ -2029,20 +2033,20 @@
         <v>32</v>
       </c>
       <c r="C28" s="22"/>
-      <c r="D28" s="64" t="s">
+      <c r="D28" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E28" s="65"/>
-      <c r="F28" s="65"/>
-      <c r="G28" s="65"/>
-      <c r="H28" s="65"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="65"/>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="66"/>
+      <c r="E28" s="67"/>
+      <c r="F28" s="67"/>
+      <c r="G28" s="67"/>
+      <c r="H28" s="67"/>
+      <c r="I28" s="67"/>
+      <c r="J28" s="67"/>
+      <c r="K28" s="67"/>
+      <c r="L28" s="67"/>
+      <c r="M28" s="67"/>
+      <c r="N28" s="67"/>
+      <c r="O28" s="68"/>
       <c r="P28" s="38"/>
       <c r="Q28" s="38"/>
       <c r="R28" s="38"/>
@@ -2063,20 +2067,20 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C29" s="22"/>
-      <c r="D29" s="64" t="s">
+      <c r="D29" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="65"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="66"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="67"/>
+      <c r="G29" s="67"/>
+      <c r="H29" s="67"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="67"/>
+      <c r="K29" s="67"/>
+      <c r="L29" s="67"/>
+      <c r="M29" s="67"/>
+      <c r="N29" s="67"/>
+      <c r="O29" s="68"/>
       <c r="P29" s="38"/>
       <c r="Q29" s="38"/>
       <c r="R29" s="38"/>
@@ -2095,20 +2099,20 @@
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="26"/>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
-      <c r="O30" s="69"/>
+      <c r="E30" s="70"/>
+      <c r="F30" s="70"/>
+      <c r="G30" s="70"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="70"/>
+      <c r="J30" s="70"/>
+      <c r="K30" s="70"/>
+      <c r="L30" s="70"/>
+      <c r="M30" s="70"/>
+      <c r="N30" s="70"/>
+      <c r="O30" s="71"/>
       <c r="P30" s="39"/>
       <c r="Q30" s="39"/>
       <c r="R30" s="39"/>
@@ -2129,20 +2133,20 @@
         <v>76</v>
       </c>
       <c r="C31" s="26"/>
-      <c r="D31" s="44" t="s">
+      <c r="D31" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="46"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="47"/>
+      <c r="J31" s="47"/>
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="47"/>
+      <c r="O31" s="48"/>
       <c r="P31" s="39"/>
       <c r="Q31" s="39"/>
       <c r="R31" s="39"/>
@@ -2165,20 +2169,20 @@
       <c r="C32" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D32" s="44" t="s">
+      <c r="D32" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="46"/>
+      <c r="E32" s="47"/>
+      <c r="F32" s="47"/>
+      <c r="G32" s="47"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="47"/>
+      <c r="J32" s="47"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="47"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="47"/>
+      <c r="O32" s="48"/>
       <c r="P32" s="39"/>
       <c r="Q32" s="39"/>
       <c r="R32" s="39"/>
@@ -2201,20 +2205,20 @@
       <c r="C33" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D33" s="44" t="s">
+      <c r="D33" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="46"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="47"/>
+      <c r="O33" s="48"/>
       <c r="P33" s="39"/>
       <c r="Q33" s="39"/>
       <c r="R33" s="39"/>
@@ -2237,20 +2241,20 @@
       <c r="C34" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="44" t="s">
+      <c r="D34" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="46"/>
+      <c r="E34" s="47"/>
+      <c r="F34" s="47"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="47"/>
+      <c r="J34" s="47"/>
+      <c r="K34" s="47"/>
+      <c r="L34" s="47"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="47"/>
+      <c r="O34" s="48"/>
       <c r="P34" s="39"/>
       <c r="Q34" s="39"/>
       <c r="R34" s="39"/>
@@ -2271,20 +2275,20 @@
         <v>77</v>
       </c>
       <c r="C35" s="26"/>
-      <c r="D35" s="44" t="s">
+      <c r="D35" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="46"/>
+      <c r="E35" s="47"/>
+      <c r="F35" s="47"/>
+      <c r="G35" s="47"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="47"/>
+      <c r="J35" s="47"/>
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="47"/>
+      <c r="O35" s="48"/>
       <c r="P35" s="39"/>
       <c r="Q35" s="39"/>
       <c r="R35" s="39"/>
@@ -2307,20 +2311,20 @@
       <c r="C36" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="44" t="s">
+      <c r="D36" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="46"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="48"/>
       <c r="P36" s="39"/>
       <c r="Q36" s="39"/>
       <c r="R36" s="39"/>
@@ -2343,20 +2347,20 @@
       <c r="C37" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D37" s="44" t="s">
+      <c r="D37" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E37" s="45"/>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="45"/>
-      <c r="I37" s="45"/>
-      <c r="J37" s="45"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="46"/>
+      <c r="E37" s="47"/>
+      <c r="F37" s="47"/>
+      <c r="G37" s="47"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="47"/>
+      <c r="J37" s="47"/>
+      <c r="K37" s="47"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="47"/>
+      <c r="O37" s="48"/>
       <c r="P37" s="39"/>
       <c r="Q37" s="39"/>
       <c r="R37" s="39"/>
@@ -2379,20 +2383,20 @@
       <c r="C38" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="44" t="s">
+      <c r="D38" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="46"/>
+      <c r="E38" s="47"/>
+      <c r="F38" s="47"/>
+      <c r="G38" s="47"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="47"/>
+      <c r="J38" s="47"/>
+      <c r="K38" s="47"/>
+      <c r="L38" s="47"/>
+      <c r="M38" s="47"/>
+      <c r="N38" s="47"/>
+      <c r="O38" s="48"/>
       <c r="P38" s="39"/>
       <c r="Q38" s="39"/>
       <c r="R38" s="39"/>
@@ -2413,20 +2417,20 @@
         <v>78</v>
       </c>
       <c r="C39" s="25"/>
-      <c r="D39" s="44" t="s">
+      <c r="D39" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="46"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
+      <c r="K39" s="47"/>
+      <c r="L39" s="47"/>
+      <c r="M39" s="47"/>
+      <c r="N39" s="47"/>
+      <c r="O39" s="48"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="39"/>
       <c r="R39" s="39"/>
@@ -2449,20 +2453,20 @@
       <c r="C40" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D40" s="44" t="s">
+      <c r="D40" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="46"/>
+      <c r="E40" s="47"/>
+      <c r="F40" s="47"/>
+      <c r="G40" s="47"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="47"/>
+      <c r="J40" s="47"/>
+      <c r="K40" s="47"/>
+      <c r="L40" s="47"/>
+      <c r="M40" s="47"/>
+      <c r="N40" s="47"/>
+      <c r="O40" s="48"/>
       <c r="P40" s="39"/>
       <c r="Q40" s="39"/>
       <c r="R40" s="39"/>
@@ -2485,20 +2489,20 @@
       <c r="C41" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D41" s="44" t="s">
+      <c r="D41" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="46"/>
+      <c r="E41" s="47"/>
+      <c r="F41" s="47"/>
+      <c r="G41" s="47"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="47"/>
+      <c r="J41" s="47"/>
+      <c r="K41" s="47"/>
+      <c r="L41" s="47"/>
+      <c r="M41" s="47"/>
+      <c r="N41" s="47"/>
+      <c r="O41" s="48"/>
       <c r="P41" s="39"/>
       <c r="Q41" s="39"/>
       <c r="R41" s="39"/>
@@ -2521,20 +2525,20 @@
       <c r="C42" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D42" s="44" t="s">
+      <c r="D42" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="46"/>
+      <c r="E42" s="47"/>
+      <c r="F42" s="47"/>
+      <c r="G42" s="47"/>
+      <c r="H42" s="47"/>
+      <c r="I42" s="47"/>
+      <c r="J42" s="47"/>
+      <c r="K42" s="47"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="48"/>
       <c r="P42" s="39"/>
       <c r="Q42" s="39"/>
       <c r="R42" s="39"/>
@@ -2555,20 +2559,20 @@
         <v>79</v>
       </c>
       <c r="C43" s="25"/>
-      <c r="D43" s="44" t="s">
+      <c r="D43" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="46"/>
+      <c r="E43" s="47"/>
+      <c r="F43" s="47"/>
+      <c r="G43" s="47"/>
+      <c r="H43" s="47"/>
+      <c r="I43" s="47"/>
+      <c r="J43" s="47"/>
+      <c r="K43" s="47"/>
+      <c r="L43" s="47"/>
+      <c r="M43" s="47"/>
+      <c r="N43" s="47"/>
+      <c r="O43" s="48"/>
       <c r="P43" s="39"/>
       <c r="Q43" s="39"/>
       <c r="R43" s="39"/>
@@ -2591,20 +2595,20 @@
       <c r="C44" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E44" s="45"/>
-      <c r="F44" s="45"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="45"/>
-      <c r="I44" s="45"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="45"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="46"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="47"/>
+      <c r="G44" s="47"/>
+      <c r="H44" s="47"/>
+      <c r="I44" s="47"/>
+      <c r="J44" s="47"/>
+      <c r="K44" s="47"/>
+      <c r="L44" s="47"/>
+      <c r="M44" s="47"/>
+      <c r="N44" s="47"/>
+      <c r="O44" s="48"/>
       <c r="P44" s="39"/>
       <c r="Q44" s="39"/>
       <c r="R44" s="39"/>
@@ -2627,20 +2631,20 @@
       <c r="C45" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D45" s="44" t="s">
+      <c r="D45" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="45"/>
-      <c r="M45" s="45"/>
-      <c r="N45" s="45"/>
-      <c r="O45" s="46"/>
+      <c r="E45" s="47"/>
+      <c r="F45" s="47"/>
+      <c r="G45" s="47"/>
+      <c r="H45" s="47"/>
+      <c r="I45" s="47"/>
+      <c r="J45" s="47"/>
+      <c r="K45" s="47"/>
+      <c r="L45" s="47"/>
+      <c r="M45" s="47"/>
+      <c r="N45" s="47"/>
+      <c r="O45" s="48"/>
       <c r="P45" s="39"/>
       <c r="Q45" s="39"/>
       <c r="R45" s="39"/>
@@ -2663,20 +2667,20 @@
       <c r="C46" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D46" s="44" t="s">
+      <c r="D46" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E46" s="45"/>
-      <c r="F46" s="45"/>
-      <c r="G46" s="45"/>
-      <c r="H46" s="45"/>
-      <c r="I46" s="45"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="45"/>
-      <c r="M46" s="45"/>
-      <c r="N46" s="45"/>
-      <c r="O46" s="46"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="47"/>
+      <c r="L46" s="47"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="47"/>
+      <c r="O46" s="48"/>
       <c r="P46" s="39"/>
       <c r="Q46" s="39"/>
       <c r="R46" s="39"/>
@@ -2697,20 +2701,20 @@
         <v>80</v>
       </c>
       <c r="C47" s="25"/>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="45"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="45"/>
-      <c r="M47" s="45"/>
-      <c r="N47" s="45"/>
-      <c r="O47" s="46"/>
+      <c r="E47" s="47"/>
+      <c r="F47" s="47"/>
+      <c r="G47" s="47"/>
+      <c r="H47" s="47"/>
+      <c r="I47" s="47"/>
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="47"/>
+      <c r="N47" s="47"/>
+      <c r="O47" s="48"/>
       <c r="P47" s="39"/>
       <c r="Q47" s="39"/>
       <c r="R47" s="39"/>
@@ -2733,20 +2737,20 @@
       <c r="C48" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D48" s="44" t="s">
+      <c r="D48" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="45"/>
-      <c r="M48" s="45"/>
-      <c r="N48" s="45"/>
-      <c r="O48" s="46"/>
+      <c r="E48" s="47"/>
+      <c r="F48" s="47"/>
+      <c r="G48" s="47"/>
+      <c r="H48" s="47"/>
+      <c r="I48" s="47"/>
+      <c r="J48" s="47"/>
+      <c r="K48" s="47"/>
+      <c r="L48" s="47"/>
+      <c r="M48" s="47"/>
+      <c r="N48" s="47"/>
+      <c r="O48" s="48"/>
       <c r="P48" s="39"/>
       <c r="Q48" s="39"/>
       <c r="R48" s="39"/>
@@ -2769,20 +2773,20 @@
       <c r="C49" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="D49" s="44" t="s">
+      <c r="D49" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="45"/>
-      <c r="M49" s="45"/>
-      <c r="N49" s="45"/>
-      <c r="O49" s="46"/>
+      <c r="E49" s="47"/>
+      <c r="F49" s="47"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="47"/>
+      <c r="I49" s="47"/>
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="47"/>
+      <c r="N49" s="47"/>
+      <c r="O49" s="48"/>
       <c r="P49" s="39"/>
       <c r="Q49" s="39"/>
       <c r="R49" s="39"/>
@@ -2805,20 +2809,20 @@
       <c r="C50" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="D50" s="44" t="s">
+      <c r="D50" s="46" t="s">
         <v>65</v>
       </c>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
-      <c r="H50" s="45"/>
-      <c r="I50" s="45"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="45"/>
-      <c r="L50" s="45"/>
-      <c r="M50" s="45"/>
-      <c r="N50" s="45"/>
-      <c r="O50" s="46"/>
+      <c r="E50" s="47"/>
+      <c r="F50" s="47"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="47"/>
+      <c r="I50" s="47"/>
+      <c r="J50" s="47"/>
+      <c r="K50" s="47"/>
+      <c r="L50" s="47"/>
+      <c r="M50" s="47"/>
+      <c r="N50" s="47"/>
+      <c r="O50" s="48"/>
       <c r="P50" s="39"/>
       <c r="Q50" s="39"/>
       <c r="R50" s="39"/>
@@ -2837,18 +2841,18 @@
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="30"/>
-      <c r="D51" s="47"/>
-      <c r="E51" s="48"/>
-      <c r="F51" s="48"/>
-      <c r="G51" s="48"/>
-      <c r="H51" s="48"/>
-      <c r="I51" s="48"/>
-      <c r="J51" s="48"/>
-      <c r="K51" s="48"/>
-      <c r="L51" s="48"/>
-      <c r="M51" s="48"/>
-      <c r="N51" s="48"/>
-      <c r="O51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="50"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="50"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="50"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="50"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="51"/>
       <c r="P51" s="40"/>
       <c r="Q51" s="40"/>
       <c r="R51" s="40"/>
@@ -2869,20 +2873,20 @@
         <v>82</v>
       </c>
       <c r="C52" s="29"/>
-      <c r="D52" s="50" t="s">
+      <c r="D52" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="51"/>
-      <c r="I52" s="51"/>
-      <c r="J52" s="51"/>
-      <c r="K52" s="51"/>
-      <c r="L52" s="51"/>
-      <c r="M52" s="51"/>
-      <c r="N52" s="51"/>
-      <c r="O52" s="52"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="53"/>
+      <c r="H52" s="53"/>
+      <c r="I52" s="53"/>
+      <c r="J52" s="53"/>
+      <c r="K52" s="53"/>
+      <c r="L52" s="53"/>
+      <c r="M52" s="53"/>
+      <c r="N52" s="53"/>
+      <c r="O52" s="54"/>
       <c r="P52" s="40"/>
       <c r="Q52" s="40"/>
       <c r="R52" s="40"/>
@@ -2897,22 +2901,22 @@
     </row>
     <row r="53" spans="1:26" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="1"/>
-      <c r="D53" s="53"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="54"/>
-      <c r="J53" s="54"/>
-      <c r="K53" s="54"/>
-      <c r="L53" s="54"/>
-      <c r="M53" s="54"/>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
+      <c r="D53" s="55"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
+      <c r="J53" s="56"/>
+      <c r="K53" s="56"/>
+      <c r="L53" s="56"/>
+      <c r="M53" s="56"/>
+      <c r="N53" s="56"/>
+      <c r="O53" s="56"/>
       <c r="P53" s="36"/>
       <c r="Q53" s="36"/>
       <c r="R53" s="36"/>
@@ -2927,26 +2931,26 @@
     </row>
     <row r="54" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="12" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B54" s="41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="C54" s="12"/>
-      <c r="D54" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="E54" s="43"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="43"/>
-      <c r="H54" s="43"/>
-      <c r="I54" s="43"/>
-      <c r="J54" s="43"/>
-      <c r="K54" s="43"/>
-      <c r="L54" s="43"/>
-      <c r="M54" s="43"/>
-      <c r="N54" s="43"/>
-      <c r="O54" s="43"/>
+      <c r="D54" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E54" s="45"/>
+      <c r="F54" s="45"/>
+      <c r="G54" s="45"/>
+      <c r="H54" s="45"/>
+      <c r="I54" s="45"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="45"/>
+      <c r="L54" s="45"/>
+      <c r="M54" s="45"/>
+      <c r="N54" s="45"/>
+      <c r="O54" s="45"/>
       <c r="P54" s="36"/>
       <c r="Q54" s="36"/>
       <c r="R54" s="36"/>
@@ -2961,28 +2965,28 @@
     </row>
     <row r="55" spans="1:26" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A55" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B55" s="34" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C55" s="12"/>
-      <c r="D55" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="43"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="43"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="43"/>
+      <c r="D55" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="45"/>
+      <c r="F55" s="45"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="45"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="45"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="45"/>
+      <c r="M55" s="45"/>
+      <c r="N55" s="45"/>
+      <c r="O55" s="45"/>
       <c r="P55" s="36" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="Q55" s="36"/>
       <c r="R55" s="36"/>
@@ -2997,16 +3001,16 @@
     </row>
     <row r="56" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C56" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E56" s="18"/>
       <c r="F56" s="18"/>
@@ -3033,16 +3037,16 @@
     </row>
     <row r="57" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A57" s="17" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D57" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E57" s="18"/>
       <c r="F57" s="18"/>
@@ -3069,7 +3073,7 @@
     </row>
     <row r="58" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A58" s="17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B58" s="18">
         <v>3696</v>
@@ -3105,7 +3109,7 @@
     </row>
     <row r="59" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A59" s="17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B59" s="18">
         <v>1308</v>
@@ -3141,16 +3145,16 @@
     </row>
     <row r="60" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="17" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D60" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E60" s="18"/>
       <c r="F60" s="18"/>
@@ -3177,7 +3181,7 @@
     </row>
     <row r="61" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A61" s="17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B61" s="18">
         <v>3169</v>
@@ -3213,7 +3217,7 @@
     </row>
     <row r="62" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A62" s="17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B62" s="18">
         <v>1181</v>
@@ -3249,16 +3253,16 @@
     </row>
     <row r="63" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A63" s="17" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B63" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C63" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D63" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E63" s="18"/>
       <c r="F63" s="18"/>
@@ -3285,7 +3289,7 @@
     </row>
     <row r="64" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B64" s="18">
         <v>3156</v>
@@ -3321,7 +3325,7 @@
     </row>
     <row r="65" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B65" s="18">
         <v>1131</v>
@@ -3357,16 +3361,16 @@
     </row>
     <row r="66" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="17" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C66" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D66" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E66" s="18"/>
       <c r="F66" s="18"/>
@@ -3393,7 +3397,7 @@
     </row>
     <row r="67" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A67" s="17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B67" s="18">
         <v>3177</v>
@@ -3429,7 +3433,7 @@
     </row>
     <row r="68" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A68" s="17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B68" s="18">
         <v>1191</v>
@@ -3465,16 +3469,16 @@
     </row>
     <row r="69" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A69" s="17" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B69" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C69" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E69" s="18"/>
       <c r="F69" s="18"/>
@@ -3501,7 +3505,7 @@
     </row>
     <row r="70" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A70" s="17" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B70" s="18">
         <v>3265</v>
@@ -3537,7 +3541,7 @@
     </row>
     <row r="71" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A71" s="17" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B71" s="18">
         <v>1153</v>
@@ -3573,16 +3577,16 @@
     </row>
     <row r="72" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A72" s="11" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B72" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C72" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E72" s="18"/>
       <c r="F72" s="18"/>
@@ -3597,7 +3601,7 @@
     </row>
     <row r="73" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A73" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B73" s="18">
         <v>3265</v>
@@ -3621,7 +3625,7 @@
     </row>
     <row r="74" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B74" s="18">
         <v>1153</v>
@@ -3645,16 +3649,16 @@
     </row>
     <row r="75" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A75" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="B75" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C75" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E75" s="18"/>
       <c r="F75" s="18"/>
@@ -3669,7 +3673,7 @@
     </row>
     <row r="76" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B76" s="18">
         <v>3224</v>
@@ -3693,7 +3697,7 @@
     </row>
     <row r="77" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A77" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B77" s="18">
         <v>1183</v>
@@ -3717,16 +3721,16 @@
     </row>
     <row r="78" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A78" s="11" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C78" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E78" s="18"/>
       <c r="F78" s="18"/>
@@ -3741,7 +3745,7 @@
     </row>
     <row r="79" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A79" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B79" s="18">
         <v>3393</v>
@@ -3765,7 +3769,7 @@
     </row>
     <row r="80" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A80" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B80" s="18">
         <v>1057</v>
@@ -3789,16 +3793,16 @@
     </row>
     <row r="81" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A81" s="11" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B81" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C81" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E81" s="18"/>
       <c r="F81" s="18"/>
@@ -3813,7 +3817,7 @@
     </row>
     <row r="82" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A82" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B82" s="18">
         <v>3282</v>
@@ -3837,7 +3841,7 @@
     </row>
     <row r="83" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B83" s="18">
         <v>1159</v>
@@ -3861,16 +3865,16 @@
     </row>
     <row r="84" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="11" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B84" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C84" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E84" s="18"/>
       <c r="F84" s="18"/>
@@ -3885,7 +3889,7 @@
     </row>
     <row r="85" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B85" s="18">
         <v>3247</v>
@@ -3909,7 +3913,7 @@
     </row>
     <row r="86" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B86" s="18">
         <v>1133</v>
@@ -3933,16 +3937,16 @@
     </row>
     <row r="87" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A87" s="11" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B87" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C87" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D87" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E87" s="18"/>
       <c r="F87" s="18"/>
@@ -3957,7 +3961,7 @@
     </row>
     <row r="88" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A88" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B88" s="18">
         <v>3249</v>
@@ -3981,7 +3985,7 @@
     </row>
     <row r="89" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B89" s="18">
         <v>1182</v>
@@ -4005,16 +4009,16 @@
     </row>
     <row r="90" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A90" s="11" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B90" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C90" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D90" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E90" s="18"/>
       <c r="F90" s="18"/>
@@ -4029,7 +4033,7 @@
     </row>
     <row r="91" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B91" s="18">
         <v>3178</v>
@@ -4053,7 +4057,7 @@
     </row>
     <row r="92" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B92" s="18">
         <v>1189</v>
@@ -4077,16 +4081,16 @@
     </row>
     <row r="93" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C93" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D93" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E93" s="18"/>
       <c r="F93" s="18"/>
@@ -4101,7 +4105,7 @@
     </row>
     <row r="94" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B94" s="18">
         <v>3324</v>
@@ -4125,7 +4129,7 @@
     </row>
     <row r="95" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B95" s="18">
         <v>871</v>
@@ -4149,16 +4153,16 @@
     </row>
     <row r="96" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="11" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B96" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C96" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D96" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E96" s="18"/>
       <c r="F96" s="18"/>
@@ -4173,7 +4177,7 @@
     </row>
     <row r="97" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B97" s="18">
         <v>3410</v>
@@ -4197,7 +4201,7 @@
     </row>
     <row r="98" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A98" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B98" s="18">
         <v>1142</v>
@@ -4221,16 +4225,16 @@
     </row>
     <row r="99" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A99" s="11" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B99" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C99" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D99" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E99" s="18"/>
       <c r="F99" s="18"/>
@@ -4245,7 +4249,7 @@
     </row>
     <row r="100" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A100" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B100" s="18">
         <v>3131</v>
@@ -4269,7 +4273,7 @@
     </row>
     <row r="101" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A101" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B101" s="18">
         <v>1170</v>
@@ -4293,16 +4297,16 @@
     </row>
     <row r="102" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="11" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B102" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C102" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E102" s="18"/>
       <c r="F102" s="18"/>
@@ -4317,7 +4321,7 @@
     </row>
     <row r="103" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A103" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B103" s="18">
         <v>3311</v>
@@ -4341,7 +4345,7 @@
     </row>
     <row r="104" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B104" s="18">
         <v>1102</v>
@@ -4365,21 +4369,21 @@
     </row>
     <row r="105" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A105" s="11" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B105" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D105" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A106" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B106" s="11">
         <v>3693</v>
@@ -4393,7 +4397,7 @@
     </row>
     <row r="107" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A107" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B107" s="11">
         <v>645</v>
@@ -4407,21 +4411,21 @@
     </row>
     <row r="108" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A108" s="11" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A109" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B109" s="11">
         <v>2709</v>
@@ -4435,7 +4439,7 @@
     </row>
     <row r="110" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A110" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B110" s="11">
         <v>925</v>
@@ -4449,21 +4453,21 @@
     </row>
     <row r="111" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A111" s="11" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D111" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A112" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B112" s="11">
         <v>3813</v>
@@ -4477,7 +4481,7 @@
     </row>
     <row r="113" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A113" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B113" s="11">
         <v>598</v>
@@ -4491,21 +4495,21 @@
     </row>
     <row r="114" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A114" s="11" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B114" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C114" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D114" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A115" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B115" s="11">
         <v>3341</v>
@@ -4519,7 +4523,7 @@
     </row>
     <row r="116" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A116" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B116" s="11">
         <v>1098</v>
@@ -4533,21 +4537,21 @@
     </row>
     <row r="117" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A117" s="11" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B117" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C117" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A118" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B118" s="11">
         <v>4133</v>
@@ -4561,7 +4565,7 @@
     </row>
     <row r="119" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A119" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B119" s="11">
         <v>1105</v>
@@ -4575,21 +4579,21 @@
     </row>
     <row r="120" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A120" s="11" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B120" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C120" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D120" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A121" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B121" s="11">
         <v>3472</v>
@@ -4603,7 +4607,7 @@
     </row>
     <row r="122" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A122" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B122" s="11">
         <v>796</v>
@@ -4617,21 +4621,21 @@
     </row>
     <row r="123" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A123" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B123" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C123" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D123" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A124" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B124" s="11">
         <v>3325</v>
@@ -4645,7 +4649,7 @@
     </row>
     <row r="125" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A125" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B125" s="11">
         <v>871</v>
@@ -4659,21 +4663,21 @@
     </row>
     <row r="126" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A126" s="11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B126" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C126" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D126" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A127" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B127" s="11">
         <v>3209</v>
@@ -4687,7 +4691,7 @@
     </row>
     <row r="128" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A128" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B128" s="11">
         <v>703</v>
@@ -4701,21 +4705,21 @@
     </row>
     <row r="129" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="11" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B129" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C129" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D129" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A130" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B130" s="11">
         <v>2947</v>
@@ -4729,7 +4733,7 @@
     </row>
     <row r="131" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A131" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B131" s="11">
         <v>797</v>
@@ -4743,21 +4747,21 @@
     </row>
     <row r="132" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A132" s="11" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B132" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C132" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D132" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A133" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B133" s="11">
         <v>3727</v>
@@ -4771,7 +4775,7 @@
     </row>
     <row r="134" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A134" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B134" s="11">
         <v>1346</v>
@@ -4785,21 +4789,21 @@
     </row>
     <row r="135" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A135" s="11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B135" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C135" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D135" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A136" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B136" s="11">
         <v>3297</v>
@@ -4813,7 +4817,7 @@
     </row>
     <row r="137" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A137" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B137" s="11">
         <v>1237</v>
@@ -4827,21 +4831,21 @@
     </row>
     <row r="138" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A138" s="11" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B138" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C138" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D138" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A139" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B139" s="11">
         <v>3280</v>
@@ -4855,7 +4859,7 @@
     </row>
     <row r="140" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A140" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B140" s="11">
         <v>1110</v>
@@ -4869,21 +4873,21 @@
     </row>
     <row r="141" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A141" s="11" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B141" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D141" s="11" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="142" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A142" s="11" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B142" s="11">
         <v>3551</v>
@@ -4897,35 +4901,74 @@
     </row>
     <row r="143" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A143" s="11" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B143" s="11">
         <v>1167</v>
       </c>
       <c r="C143" s="11">
-        <v>1402</v>
+        <v>1405</v>
       </c>
       <c r="D143" s="11">
-        <v>1206</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="145" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="146" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="147" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="148" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="149" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="150" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="151" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="152" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="153" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="154" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="155" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="156" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="157" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="158" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="159" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="160" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A144" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C144" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D144" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A145" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B145" s="11">
+        <v>3247</v>
+      </c>
+      <c r="C145" s="11">
+        <v>2450</v>
+      </c>
+      <c r="D145" s="11">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A146" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B146" s="11">
+        <v>1134</v>
+      </c>
+      <c r="C146" s="11">
+        <v>1360</v>
+      </c>
+      <c r="D146" s="11">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="148" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="149" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="150" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="151" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="152" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="153" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="154" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="155" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="156" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="157" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="158" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="159" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="160" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="161" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="162" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="163" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5824,10 +5867,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD610E5-7CFE-40D9-832A-CDCE1C3A467E}">
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52:D54"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5844,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="1"/>
@@ -5863,8 +5906,8 @@
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="34">
-        <v>117409.83500000001</v>
+      <c r="B2" s="42">
+        <v>117630.98299999999</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>75</v>
@@ -5887,8 +5930,8 @@
       <c r="A3" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="34">
-        <v>560476.92599999998</v>
+      <c r="B3" s="42">
+        <v>560491.24300000002</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>75</v>
@@ -5911,8 +5954,8 @@
       <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="12">
-        <v>6.2169999999999996</v>
+      <c r="B4" s="42">
+        <v>9.24</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>74</v>
@@ -6072,7 +6115,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="16">
-        <v>-200</v>
+        <v>-400</v>
       </c>
       <c r="C11" s="16" t="s">
         <v>13</v>
@@ -6096,7 +6139,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="16">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>13</v>
@@ -6192,7 +6235,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="16">
-        <v>180</v>
+        <v>-125</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>19</v>
@@ -6216,7 +6259,7 @@
         <v>20</v>
       </c>
       <c r="B17" s="16">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>19</v>
@@ -6442,7 +6485,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C27" s="22"/>
       <c r="D27" s="24" t="s">
@@ -6528,7 +6571,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C31" s="26"/>
       <c r="D31" s="25" t="s">
@@ -6549,8 +6592,8 @@
       <c r="A32" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="33">
-        <v>117393.80899999999</v>
+      <c r="B32" s="42">
+        <v>117628.84600000001</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>75</v>
@@ -6573,8 +6616,8 @@
       <c r="A33" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="33">
-        <v>560459.92500000005</v>
+      <c r="B33" s="42">
+        <v>560479.14500000002</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>75</v>
@@ -6597,8 +6640,8 @@
       <c r="A34" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="33">
-        <v>2.282</v>
+      <c r="B34" s="42">
+        <v>6.2229999999999999</v>
       </c>
       <c r="C34" s="26" t="s">
         <v>74</v>
@@ -6622,9 +6665,9 @@
         <v>29</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="26"/>
+        <v>131</v>
+      </c>
+      <c r="C35" s="25"/>
       <c r="D35" s="25" t="s">
         <v>64</v>
       </c>
@@ -6643,8 +6686,8 @@
       <c r="A36" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B36" s="25">
-        <v>117407.497</v>
+      <c r="B36" s="42">
+        <v>117619.48699999999</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>75</v>
@@ -6667,8 +6710,8 @@
       <c r="A37" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="25">
-        <v>560459.32900000003</v>
+      <c r="B37" s="42">
+        <v>560481.81499999994</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>75</v>
@@ -6691,8 +6734,8 @@
       <c r="A38" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="25">
-        <v>2.1869999999999998</v>
+      <c r="B38" s="42">
+        <v>6.3410000000000002</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>74</v>
@@ -6716,7 +6759,7 @@
         <v>29</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>86</v>
+        <v>134</v>
       </c>
       <c r="C39" s="25"/>
       <c r="D39" s="25" t="s">
@@ -6737,8 +6780,8 @@
       <c r="A40" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B40" s="25">
-        <v>117403.439</v>
+      <c r="B40" s="42">
+        <v>117616.802</v>
       </c>
       <c r="C40" s="26" t="s">
         <v>75</v>
@@ -6761,8 +6804,8 @@
       <c r="A41" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B41" s="25">
-        <v>560459.66700000002</v>
+      <c r="B41" s="42">
+        <v>560462.995</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>75</v>
@@ -6785,8 +6828,8 @@
       <c r="A42" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="25">
-        <v>2.1819999999999999</v>
+      <c r="B42" s="42">
+        <v>2.6960000000000002</v>
       </c>
       <c r="C42" s="26" t="s">
         <v>74</v>
@@ -6810,7 +6853,7 @@
         <v>29</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>87</v>
+        <v>132</v>
       </c>
       <c r="C43" s="25"/>
       <c r="D43" s="25" t="s">
@@ -6831,8 +6874,8 @@
       <c r="A44" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B44" s="25">
-        <v>117406.65</v>
+      <c r="B44" s="42">
+        <v>117560.32799999999</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>75</v>
@@ -6855,8 +6898,8 @@
       <c r="A45" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="B45" s="25">
-        <v>560411.27800000005</v>
+      <c r="B45" s="42">
+        <v>560454.07299999997</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>75</v>
@@ -6879,8 +6922,8 @@
       <c r="A46" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="25">
-        <v>1.756</v>
+      <c r="B46" s="42">
+        <v>3.8279999999999998</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>74</v>
@@ -6921,8 +6964,8 @@
       <c r="A48" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B48" s="31" t="s">
-        <v>89</v>
+      <c r="B48" s="43" t="s">
+        <v>133</v>
       </c>
       <c r="C48" s="29"/>
       <c r="D48" s="32" t="s">
@@ -6939,81 +6982,281 @@
       <c r="M48" s="29"/>
       <c r="N48" s="29"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="26"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A52" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="C52" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D52" s="11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A53" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" s="11">
-        <v>3246</v>
-      </c>
-      <c r="C53" s="11">
-        <v>2449</v>
-      </c>
-      <c r="D53" s="11">
-        <v>2994</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A54" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B54" s="11">
-        <v>1134</v>
-      </c>
-      <c r="C54" s="11">
-        <v>1358</v>
-      </c>
-      <c r="D54" s="11">
-        <v>1173</v>
+    <row r="49" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="55"/>
+      <c r="E49" s="56"/>
+      <c r="F49" s="56"/>
+      <c r="G49" s="56"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
+      <c r="J49" s="56"/>
+      <c r="K49" s="56"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="56"/>
+      <c r="O49" s="56"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A50" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C50" s="12"/>
+      <c r="D50" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E50" s="45"/>
+      <c r="F50" s="45"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
+      <c r="K50" s="45"/>
+      <c r="L50" s="45"/>
+      <c r="M50" s="45"/>
+      <c r="N50" s="45"/>
+      <c r="O50" s="45"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A51" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E51" s="45"/>
+      <c r="F51" s="45"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="45"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="45"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="45"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="45"/>
+      <c r="O51" s="45"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A52" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E52" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A53" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="25">
+        <v>825</v>
+      </c>
+      <c r="C53" s="26">
+        <v>3032</v>
+      </c>
+      <c r="D53" s="25">
+        <v>1742</v>
+      </c>
+      <c r="E53" s="25">
+        <v>3778</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A54" t="s">
+        <v>102</v>
+      </c>
+      <c r="B54">
+        <v>2087</v>
+      </c>
+      <c r="C54">
+        <v>1924</v>
+      </c>
+      <c r="D54">
+        <v>1915</v>
+      </c>
+      <c r="E54">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A55" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B55" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A56" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="11">
+        <v>461</v>
+      </c>
+      <c r="C56" s="11">
+        <v>2688</v>
+      </c>
+      <c r="D56" s="11">
+        <v>1419</v>
+      </c>
+      <c r="E56">
+        <v>3392</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A57" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B57" s="11">
+        <v>2028</v>
+      </c>
+      <c r="C57" s="11">
+        <v>1894</v>
+      </c>
+      <c r="D57" s="11">
+        <v>1859</v>
+      </c>
+      <c r="E57">
+        <v>1540</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>100</v>
+      </c>
+      <c r="D58" t="s">
+        <v>100</v>
+      </c>
+      <c r="E58" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="B59">
+        <v>227</v>
+      </c>
+      <c r="C59">
+        <v>2533</v>
+      </c>
+      <c r="D59">
+        <v>1250</v>
+      </c>
+      <c r="E59">
+        <v>3174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60">
+        <v>2317</v>
+      </c>
+      <c r="C60">
+        <v>1983</v>
+      </c>
+      <c r="D60">
+        <v>2050</v>
+      </c>
+      <c r="E60">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A61" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E61" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62">
+        <v>475</v>
+      </c>
+      <c r="C62">
+        <v>2695</v>
+      </c>
+      <c r="D62">
+        <v>1431</v>
+      </c>
+      <c r="E62">
+        <v>3405</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63">
+        <v>1975</v>
+      </c>
+      <c r="C63">
+        <v>1857</v>
+      </c>
+      <c r="D63">
+        <v>1814</v>
+      </c>
+      <c r="E63">
+        <v>1507</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D49:O49"/>
+    <mergeCell ref="D50:O50"/>
+    <mergeCell ref="D51:O51"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Functional PettenNoord and Texel
</commit_message>
<xml_diff>
--- a/Database/CoastSnapPyDB.xlsx
+++ b/Database/CoastSnapPyDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathvansoest/Documents/CoastSnapPy/Database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D556D7A-5883-3D4B-B0CD-1B96AC0F7C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA2D8C0-15CE-1C40-A9DB-A25D84DA1AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="egmond" sheetId="10" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="139">
   <si>
     <t>Station Data</t>
   </si>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C82C2A5-FA5F-4BBC-B066-D9DA22911E90}">
   <dimension ref="A1:Z993"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -5892,8 +5892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DD610E5-7CFE-40D9-832A-CDCE1C3A467E}">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A64" sqref="A64:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5910,7 +5910,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="1"/>
@@ -7286,9 +7286,1672 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9041922D-43FF-BC4F-BA23-7B394027D7C4}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="54.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="31" customWidth="1"/>
+    <col min="5" max="5" width="42" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="10"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11">
+        <v>105850.868</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="11">
+        <v>532033.92500000005</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="11">
+        <v>25.713999999999999</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="14">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="12">
+        <v>2</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A11" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="16">
+        <v>-400</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="17"/>
+      <c r="F11" s="17"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="16">
+        <v>600</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="17"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="17"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A13" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="16">
+        <v>100</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
+      <c r="N13" s="17"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A14" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1700</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A15" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="17"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="16">
+        <v>-10</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="17"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A17" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="16">
+        <v>87</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="17"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A18" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="16">
+        <v>0</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A19" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="16">
+        <v>40</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A20" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="16">
+        <v>70</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="17"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A21" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="16">
+        <v>10</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="17"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="17"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A22" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="16">
+        <v>0.1</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+    </row>
+    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A24" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A25" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+    </row>
+    <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A27" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="22"/>
+      <c r="D27" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="24"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A28" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="24"/>
+      <c r="F28" s="24"/>
+      <c r="G28" s="24"/>
+      <c r="H28" s="24"/>
+      <c r="I28" s="24"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
+      <c r="N28" s="24"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A29" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="23">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C29" s="22"/>
+      <c r="D29" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
+      <c r="H30" s="25"/>
+      <c r="I30" s="25"/>
+      <c r="J30" s="25"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="25"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A31" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="25"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="25"/>
+      <c r="K31" s="25"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="25"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A32" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="11">
+        <v>105863.44100000001</v>
+      </c>
+      <c r="C32" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D32" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E32" s="25"/>
+      <c r="F32" s="25"/>
+      <c r="G32" s="25"/>
+      <c r="H32" s="25"/>
+      <c r="I32" s="25"/>
+      <c r="J32" s="25"/>
+      <c r="K32" s="25"/>
+      <c r="L32" s="25"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="25"/>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A33" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" s="11">
+        <v>532171.375</v>
+      </c>
+      <c r="C33" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="25"/>
+      <c r="L33" s="25"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="25"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A34" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="11">
+        <v>5.67</v>
+      </c>
+      <c r="C34" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E34" s="25"/>
+      <c r="F34" s="25"/>
+      <c r="G34" s="25"/>
+      <c r="H34" s="25"/>
+      <c r="I34" s="25"/>
+      <c r="J34" s="25"/>
+      <c r="K34" s="25"/>
+      <c r="L34" s="25"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="25"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A35" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="26"/>
+      <c r="D35" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E35" s="25"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
+      <c r="I35" s="25"/>
+      <c r="J35" s="25"/>
+      <c r="K35" s="25"/>
+      <c r="L35" s="25"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="25"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A36" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="11">
+        <v>105860.08100000001</v>
+      </c>
+      <c r="C36" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E36" s="25"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="25"/>
+      <c r="J36" s="25"/>
+      <c r="K36" s="25"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="25"/>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A37" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="11">
+        <v>532182.11199999996</v>
+      </c>
+      <c r="C37" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="25"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="25"/>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="25"/>
+      <c r="L37" s="25"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="25"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A38" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="11">
+        <v>5.952</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
+      <c r="M38" s="25"/>
+      <c r="N38" s="25"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A39" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="C39" s="26"/>
+      <c r="D39" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="25"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A40" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="11">
+        <v>105851.28599999999</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="25"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A41" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B41" s="11">
+        <v>532182.00699999998</v>
+      </c>
+      <c r="C41" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="25"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A42" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="11">
+        <v>5.2169999999999996</v>
+      </c>
+      <c r="C42" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="25"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A43" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B43" s="48" t="s">
+        <v>136</v>
+      </c>
+      <c r="C43" s="26"/>
+      <c r="D43" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="25"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A44" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B44" s="11">
+        <v>105831.228</v>
+      </c>
+      <c r="C44" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D44" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="25"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A45" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B45" s="11">
+        <v>532265.55299999996</v>
+      </c>
+      <c r="C45" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="25"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A46" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46" s="11">
+        <v>4.7960000000000003</v>
+      </c>
+      <c r="C46" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="25"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A47" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="26"/>
+      <c r="D47" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="25"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A48" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B48" s="11">
+        <v>105901.41</v>
+      </c>
+      <c r="C48" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D48" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="25"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A49" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="11">
+        <v>532291.62699999998</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="25"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A50" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50" s="11">
+        <v>4.76</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="25"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A51" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="26"/>
+      <c r="D51" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="25"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A52" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B52" s="11">
+        <v>105916.59299999999</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D52" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="25"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A53" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="11">
+        <v>532348.30200000003</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="25"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A54" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="11">
+        <v>3.3330000000000002</v>
+      </c>
+      <c r="C54" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="D54" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="25"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A55" s="29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="C55" s="29"/>
+      <c r="D55" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="29"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="29"/>
+      <c r="I55" s="29"/>
+      <c r="J55" s="29"/>
+      <c r="K55" s="29"/>
+      <c r="L55" s="29"/>
+      <c r="M55" s="29"/>
+      <c r="N55" s="29"/>
+    </row>
+    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="46"/>
+      <c r="E56" s="47"/>
+      <c r="F56" s="47"/>
+      <c r="G56" s="47"/>
+      <c r="H56" s="47"/>
+      <c r="I56" s="47"/>
+      <c r="J56" s="47"/>
+      <c r="K56" s="47"/>
+      <c r="L56" s="47"/>
+      <c r="M56" s="47"/>
+      <c r="N56" s="47"/>
+      <c r="O56" s="47"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A57" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C57" s="12"/>
+      <c r="D57" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="E57" s="45"/>
+      <c r="F57" s="45"/>
+      <c r="G57" s="45"/>
+      <c r="H57" s="45"/>
+      <c r="I57" s="45"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="45"/>
+      <c r="L57" s="45"/>
+      <c r="M57" s="45"/>
+      <c r="N57" s="45"/>
+      <c r="O57" s="45"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A58" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B58" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="45"/>
+      <c r="H58" s="45"/>
+      <c r="I58" s="45"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="45"/>
+      <c r="L58" s="45"/>
+      <c r="M58" s="45"/>
+      <c r="N58" s="45"/>
+      <c r="O58" s="45"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A59" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C59" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="D59" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="E59" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A60" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="25">
+        <v>2205</v>
+      </c>
+      <c r="C60" s="26">
+        <v>1676</v>
+      </c>
+      <c r="D60" s="25">
+        <v>2522</v>
+      </c>
+      <c r="E60" s="25">
+        <v>2561</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61">
+        <v>1502</v>
+      </c>
+      <c r="C61">
+        <v>1345</v>
+      </c>
+      <c r="D61">
+        <v>1308</v>
+      </c>
+      <c r="E61">
+        <v>1276</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A62" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B62" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E62" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A63" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="11">
+        <v>1791</v>
+      </c>
+      <c r="C63" s="11">
+        <v>1225</v>
+      </c>
+      <c r="D63" s="11">
+        <v>2098</v>
+      </c>
+      <c r="E63">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
+      <c r="A64" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B64" s="11">
+        <v>1376</v>
+      </c>
+      <c r="C64" s="11">
+        <v>1224</v>
+      </c>
+      <c r="D64" s="11">
+        <v>1174</v>
+      </c>
+      <c r="E64">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A65" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" t="s">
+        <v>100</v>
+      </c>
+      <c r="C65" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>100</v>
+      </c>
+      <c r="E65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A66" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66">
+        <v>1547</v>
+      </c>
+      <c r="C66">
+        <v>986</v>
+      </c>
+      <c r="D66">
+        <v>1841</v>
+      </c>
+      <c r="E66">
+        <v>1876</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A67" t="s">
+        <v>102</v>
+      </c>
+      <c r="B67">
+        <v>1422</v>
+      </c>
+      <c r="C67">
+        <v>1285</v>
+      </c>
+      <c r="D67">
+        <v>1220</v>
+      </c>
+      <c r="E67">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A68" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C68" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="E68" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69">
+        <v>1693</v>
+      </c>
+      <c r="C69">
+        <v>1118</v>
+      </c>
+      <c r="D69">
+        <v>1999</v>
+      </c>
+      <c r="E69">
+        <v>2034</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A70" t="s">
+        <v>102</v>
+      </c>
+      <c r="B70">
+        <v>1375</v>
+      </c>
+      <c r="C70">
+        <v>1222</v>
+      </c>
+      <c r="D70">
+        <v>1170</v>
+      </c>
+      <c r="E70">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71" t="s">
+        <v>100</v>
+      </c>
+      <c r="C71" t="s">
+        <v>100</v>
+      </c>
+      <c r="D71" t="s">
+        <v>100</v>
+      </c>
+      <c r="E71" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A72" t="s">
+        <v>101</v>
+      </c>
+      <c r="B72">
+        <v>2795</v>
+      </c>
+      <c r="C72">
+        <v>2249</v>
+      </c>
+      <c r="D72">
+        <v>3152</v>
+      </c>
+      <c r="E72">
+        <v>3198</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A73" t="s">
+        <v>102</v>
+      </c>
+      <c r="B73">
+        <v>1399</v>
+      </c>
+      <c r="C73">
+        <v>1223</v>
+      </c>
+      <c r="D73">
+        <v>1203</v>
+      </c>
+      <c r="E73">
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A74" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" t="s">
+        <v>100</v>
+      </c>
+      <c r="D74" t="s">
+        <v>100</v>
+      </c>
+      <c r="E74" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A75" t="s">
+        <v>101</v>
+      </c>
+      <c r="B75">
+        <v>1711</v>
+      </c>
+      <c r="C75">
+        <v>1100</v>
+      </c>
+      <c r="D75">
+        <v>2040</v>
+      </c>
+      <c r="E75">
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="A76" t="s">
+        <v>102</v>
+      </c>
+      <c r="B76">
+        <v>1313</v>
+      </c>
+      <c r="C76">
+        <v>1149</v>
+      </c>
+      <c r="D76">
+        <v>1095</v>
+      </c>
+      <c r="E76">
+        <v>1061</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB696BC-751D-C645-9BC9-76CF1CF3C2E5}">
+  <dimension ref="A1:O61"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -7326,7 +8989,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="11">
-        <v>105850.868</v>
+        <v>105840.447</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>75</v>
@@ -7350,7 +9013,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="11">
-        <v>532033.92500000005</v>
+        <v>532018.59400000004</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>75</v>
@@ -7374,7 +9037,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="11">
-        <v>25.713999999999999</v>
+        <v>25.928999999999998</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>74</v>
@@ -7558,7 +9221,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="16">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C12" s="16" t="s">
         <v>13</v>
@@ -7582,7 +9245,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="16">
-        <v>100</v>
+        <v>-600</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>13</v>
@@ -7606,7 +9269,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="16">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C14" s="16" t="s">
         <v>13</v>
@@ -7654,7 +9317,7 @@
         <v>18</v>
       </c>
       <c r="B16" s="16">
-        <v>-10</v>
+        <v>-125</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>19</v>
@@ -7904,1567 +9567,6 @@
         <v>27</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>83</v>
-      </c>
-      <c r="C27" s="22"/>
-      <c r="D27" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="24"/>
-      <c r="N27" s="24"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A28" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="22"/>
-      <c r="D28" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="24"/>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A29" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="23">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C29" s="22"/>
-      <c r="D29" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="24"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="24"/>
-      <c r="N29" s="24"/>
-    </row>
-    <row r="30" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="27" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A31" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C31" s="26"/>
-      <c r="D31" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
-      <c r="L31" s="25"/>
-      <c r="M31" s="25"/>
-      <c r="N31" s="25"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A32" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B32" s="11">
-        <v>105863.44100000001</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E32" s="25"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="25"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A33" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B33" s="11">
-        <v>532171.375</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="25"/>
-      <c r="J33" s="25"/>
-      <c r="K33" s="25"/>
-      <c r="L33" s="25"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="25"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A34" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="11">
-        <v>5.67</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="25"/>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A35" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B35" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="C35" s="26"/>
-      <c r="D35" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A36" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B36" s="11">
-        <v>105860.08100000001</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="25"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A37" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B37" s="11">
-        <v>532182.11199999996</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
-      <c r="L37" s="25"/>
-      <c r="M37" s="25"/>
-      <c r="N37" s="25"/>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A38" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="11">
-        <v>5.952</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D38" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
-      <c r="M38" s="25"/>
-      <c r="N38" s="25"/>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A39" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="26"/>
-      <c r="D39" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
-      <c r="M39" s="25"/>
-      <c r="N39" s="25"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A40" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40" s="11">
-        <v>105851.28599999999</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
-      <c r="M40" s="25"/>
-      <c r="N40" s="25"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A41" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B41" s="11">
-        <v>532182.00699999998</v>
-      </c>
-      <c r="C41" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="25"/>
-      <c r="N41" s="25"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A42" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B42" s="11">
-        <v>5.2169999999999996</v>
-      </c>
-      <c r="C42" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="25"/>
-      <c r="N42" s="25"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A43" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="48" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="25"/>
-      <c r="N43" s="25"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A44" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B44" s="11">
-        <v>105831.228</v>
-      </c>
-      <c r="C44" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D44" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="25"/>
-      <c r="N44" s="25"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A45" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B45" s="11">
-        <v>532265.55299999996</v>
-      </c>
-      <c r="C45" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="25"/>
-      <c r="N45" s="25"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A46" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="11">
-        <v>4.7960000000000003</v>
-      </c>
-      <c r="C46" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="25"/>
-      <c r="N46" s="25"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A47" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B47" s="48" t="s">
-        <v>131</v>
-      </c>
-      <c r="C47" s="26"/>
-      <c r="D47" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="25"/>
-      <c r="N47" s="25"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A48" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B48" s="11">
-        <v>105901.41</v>
-      </c>
-      <c r="C48" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D48" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="25"/>
-      <c r="N48" s="25"/>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A49" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B49" s="11">
-        <v>532291.62699999998</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D49" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="25"/>
-      <c r="N49" s="25"/>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A50" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B50" s="11">
-        <v>4.76</v>
-      </c>
-      <c r="C50" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="25"/>
-      <c r="N50" s="25"/>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A51" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="B51" s="48" t="s">
-        <v>134</v>
-      </c>
-      <c r="C51" s="26"/>
-      <c r="D51" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="25"/>
-      <c r="L51" s="25"/>
-      <c r="M51" s="25"/>
-      <c r="N51" s="25"/>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A52" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="B52" s="11">
-        <v>105916.59299999999</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="25"/>
-      <c r="N52" s="25"/>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A53" s="25" t="s">
-        <v>3</v>
-      </c>
-      <c r="B53" s="11">
-        <v>532348.30200000003</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D53" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A54" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="11">
-        <v>3.3330000000000002</v>
-      </c>
-      <c r="C54" s="26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D54" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="25"/>
-      <c r="N54" s="25"/>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A55" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B55" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" s="29"/>
-      <c r="D55" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="E55" s="29"/>
-      <c r="F55" s="29"/>
-      <c r="G55" s="29"/>
-      <c r="H55" s="29"/>
-      <c r="I55" s="29"/>
-      <c r="J55" s="29"/>
-      <c r="K55" s="29"/>
-      <c r="L55" s="29"/>
-      <c r="M55" s="29"/>
-      <c r="N55" s="29"/>
-    </row>
-    <row r="56" spans="1:15" ht="21" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="47"/>
-      <c r="F56" s="47"/>
-      <c r="G56" s="47"/>
-      <c r="H56" s="47"/>
-      <c r="I56" s="47"/>
-      <c r="J56" s="47"/>
-      <c r="K56" s="47"/>
-      <c r="L56" s="47"/>
-      <c r="M56" s="47"/>
-      <c r="N56" s="47"/>
-      <c r="O56" s="47"/>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A57" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="B57" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="C57" s="12"/>
-      <c r="D57" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="45"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="45"/>
-      <c r="L57" s="45"/>
-      <c r="M57" s="45"/>
-      <c r="N57" s="45"/>
-      <c r="O57" s="45"/>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A58" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B58" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="C58" s="12"/>
-      <c r="D58" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="45"/>
-      <c r="L58" s="45"/>
-      <c r="M58" s="45"/>
-      <c r="N58" s="45"/>
-      <c r="O58" s="45"/>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A59" s="25" t="s">
-        <v>97</v>
-      </c>
-      <c r="B59" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="C59" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="D59" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="E59" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A60" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="25">
-        <v>2205</v>
-      </c>
-      <c r="C60" s="26">
-        <v>1676</v>
-      </c>
-      <c r="D60" s="25">
-        <v>2522</v>
-      </c>
-      <c r="E60" s="25">
-        <v>2561</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
-        <v>102</v>
-      </c>
-      <c r="B61">
-        <v>1502</v>
-      </c>
-      <c r="C61">
-        <v>1345</v>
-      </c>
-      <c r="D61">
-        <v>1308</v>
-      </c>
-      <c r="E61">
-        <v>1276</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A62" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B62" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E62" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A63" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B63" s="11">
-        <v>1791</v>
-      </c>
-      <c r="C63" s="11">
-        <v>1225</v>
-      </c>
-      <c r="D63" s="11">
-        <v>2098</v>
-      </c>
-      <c r="E63">
-        <v>2133</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A64" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B64" s="11">
-        <v>1376</v>
-      </c>
-      <c r="C64" s="11">
-        <v>1224</v>
-      </c>
-      <c r="D64" s="11">
-        <v>1174</v>
-      </c>
-      <c r="E64">
-        <v>1143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A65" t="s">
-        <v>96</v>
-      </c>
-      <c r="B65" t="s">
-        <v>100</v>
-      </c>
-      <c r="C65" t="s">
-        <v>100</v>
-      </c>
-      <c r="D65" t="s">
-        <v>100</v>
-      </c>
-      <c r="E65" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A66" t="s">
-        <v>101</v>
-      </c>
-      <c r="B66">
-        <v>1547</v>
-      </c>
-      <c r="C66">
-        <v>986</v>
-      </c>
-      <c r="D66">
-        <v>1841</v>
-      </c>
-      <c r="E66">
-        <v>1876</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A67" t="s">
-        <v>102</v>
-      </c>
-      <c r="B67">
-        <v>1422</v>
-      </c>
-      <c r="C67">
-        <v>1285</v>
-      </c>
-      <c r="D67">
-        <v>1220</v>
-      </c>
-      <c r="E67">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A68" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B68" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E68" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A69" t="s">
-        <v>101</v>
-      </c>
-      <c r="B69">
-        <v>1693</v>
-      </c>
-      <c r="C69">
-        <v>1118</v>
-      </c>
-      <c r="D69">
-        <v>1999</v>
-      </c>
-      <c r="E69">
-        <v>2034</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A70" t="s">
-        <v>102</v>
-      </c>
-      <c r="B70">
-        <v>1375</v>
-      </c>
-      <c r="C70">
-        <v>1222</v>
-      </c>
-      <c r="D70">
-        <v>1170</v>
-      </c>
-      <c r="E70">
-        <v>1139</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB696BC-751D-C645-9BC9-76CF1CF3C2E5}">
-  <dimension ref="A1:O61"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="28.33203125" customWidth="1"/>
-    <col min="2" max="2" width="54.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
-    <col min="4" max="4" width="31" customWidth="1"/>
-    <col min="5" max="5" width="42" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="11">
-        <v>105840.447</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="11">
-        <v>532018.59400000004</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="11">
-        <v>25.928999999999998</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-    </row>
-    <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="14">
-        <v>1</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="12">
-        <v>2</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="M10" s="17"/>
-      <c r="N10" s="17"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A11" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="16">
-        <v>-400</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="17"/>
-      <c r="N11" s="17"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A12" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="16">
-        <v>0</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="17"/>
-      <c r="N12" s="17"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A13" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="16">
-        <v>-600</v>
-      </c>
-      <c r="C13" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
-      <c r="J13" s="17"/>
-      <c r="K13" s="17"/>
-      <c r="L13" s="17"/>
-      <c r="M13" s="17"/>
-      <c r="N13" s="17"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A14" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="16">
-        <v>0</v>
-      </c>
-      <c r="C14" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
-      <c r="N14" s="17"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A15" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="C15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-      <c r="M15" s="17"/>
-      <c r="N15" s="17"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="16">
-        <v>-125</v>
-      </c>
-      <c r="C16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="17"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="16">
-        <v>87</v>
-      </c>
-      <c r="C17" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="17"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="17"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A18" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="16">
-        <v>0</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="17"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="17"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A19" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="16">
-        <v>40</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="17"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="16">
-        <v>70</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="17"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A21" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="16">
-        <v>10</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" s="17"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="17"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="17"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A22" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="16">
-        <v>0.1</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="17"/>
-    </row>
-    <row r="23" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A24" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C24" s="19"/>
-      <c r="D24" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" s="21"/>
-      <c r="F24" s="21"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
-      <c r="J24" s="21"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A25" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="21"/>
-    </row>
-    <row r="26" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7"/>
-      <c r="N26" s="7"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A27" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C27" s="22"/>

</xml_diff>